<commit_message>
Add summary, FusionChart now fills the page
</commit_message>
<xml_diff>
--- a/Archive folder/data_cleanup/deforestation_cleanup.xlsx
+++ b/Archive folder/data_cleanup/deforestation_cleanup.xlsx
@@ -772,8 +772,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1069,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N212"/>
+  <dimension ref="A1:U212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1108,7 @@
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>231</v>
       </c>
@@ -1124,7 +1152,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1168,8 +1196,16 @@
       <c r="N2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <f>CORREL(B2:B212,$J2:$J212)</f>
+        <v>0.30211839762444498</v>
+      </c>
+      <c r="Q2">
+        <f>CORREL(C2:C212,$J2:$J212)</f>
+        <v>0.29741262066619811</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1213,8 +1249,24 @@
       <c r="N3" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <f>CORREL(K2:K212,$J2:$J212)</f>
+        <v>0.14098096370238505</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:U3" si="1">CORREL(L2:L212,$J2:$J212)</f>
+        <v>8.0798327522398281E-2</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="1"/>
+        <v>0.38148870268716017</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="1"/>
+        <v>0.17113939654641497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1259,7 +1311,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1304,7 +1356,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1349,7 +1401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1394,7 +1446,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1439,7 +1491,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1484,7 +1536,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1529,7 +1581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1574,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1619,7 +1671,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1664,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1709,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1754,7 +1806,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -4033,7 +4085,7 @@
         <v>0</v>
       </c>
       <c r="J66" s="2">
-        <f t="shared" ref="J66:J128" si="1">SUM(F66:I66)</f>
+        <f t="shared" ref="J66:J128" si="2">SUM(F66:I66)</f>
         <v>20</v>
       </c>
       <c r="K66" s="1">
@@ -4078,7 +4130,7 @@
         <v>71</v>
       </c>
       <c r="J67" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="K67" s="1">
@@ -4123,7 +4175,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="K68" s="1">
@@ -4168,7 +4220,7 @@
         <v>40</v>
       </c>
       <c r="J69" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115</v>
       </c>
       <c r="K69" s="1">
@@ -4213,7 +4265,7 @@
         <v>47</v>
       </c>
       <c r="J70" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="K70" s="1">
@@ -4258,7 +4310,7 @@
         <v>162</v>
       </c>
       <c r="J71" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>259</v>
       </c>
       <c r="K71" s="1">
@@ -4303,7 +4355,7 @@
         <v>5</v>
       </c>
       <c r="J72" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="K72" s="1">
@@ -4348,7 +4400,7 @@
         <v>61</v>
       </c>
       <c r="J73" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="K73" s="1">
@@ -4393,7 +4445,7 @@
         <v>36</v>
       </c>
       <c r="J74" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="K74" s="1">
@@ -4438,7 +4490,7 @@
         <v>119</v>
       </c>
       <c r="J75" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="K75" s="1">
@@ -4483,7 +4535,7 @@
         <v>63</v>
       </c>
       <c r="J76" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>170</v>
       </c>
       <c r="K76" s="1">
@@ -4528,7 +4580,7 @@
         <v>1</v>
       </c>
       <c r="J77" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="K77" s="1">
@@ -4573,7 +4625,7 @@
         <v>3</v>
       </c>
       <c r="J78" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="K78" s="1">
@@ -4618,7 +4670,7 @@
         <v>4</v>
       </c>
       <c r="J79" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="K79" s="1">
@@ -4663,7 +4715,7 @@
         <v>101</v>
       </c>
       <c r="J80" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>167</v>
       </c>
       <c r="K80" s="1">
@@ -4708,7 +4760,7 @@
         <v>50</v>
       </c>
       <c r="J81" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>173</v>
       </c>
       <c r="K81" s="1">
@@ -4753,7 +4805,7 @@
         <v>5</v>
       </c>
       <c r="J82" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="K82" s="1">
@@ -4798,7 +4850,7 @@
         <v>26</v>
       </c>
       <c r="J83" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="K83" s="1">
@@ -4843,7 +4895,7 @@
         <v>42</v>
       </c>
       <c r="J84" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92</v>
       </c>
       <c r="K84" s="1">
@@ -4888,7 +4940,7 @@
         <v>123</v>
       </c>
       <c r="J85" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>184</v>
       </c>
       <c r="K85" s="1">
@@ -4933,7 +4985,7 @@
         <v>40</v>
       </c>
       <c r="J86" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="K86" s="1">
@@ -4978,7 +5030,7 @@
         <v>0</v>
       </c>
       <c r="J87" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="K87" s="1">
@@ -5023,7 +5075,7 @@
         <v>387</v>
       </c>
       <c r="J88" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>791</v>
       </c>
       <c r="K88" s="1">
@@ -5068,7 +5120,7 @@
         <v>428</v>
       </c>
       <c r="J89" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>930</v>
       </c>
       <c r="K89" s="1">
@@ -5113,7 +5165,7 @@
         <v>4</v>
       </c>
       <c r="J90" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>94</v>
       </c>
       <c r="K90" s="1">
@@ -5158,7 +5210,7 @@
         <v>2</v>
       </c>
       <c r="J91" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="K91" s="1">
@@ -5203,7 +5255,7 @@
         <v>3</v>
       </c>
       <c r="J92" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="K92" s="1">
@@ -5248,7 +5300,7 @@
         <v>0</v>
       </c>
       <c r="J93" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K93" s="1" t="s">
@@ -5293,7 +5345,7 @@
         <v>10</v>
       </c>
       <c r="J94" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>88</v>
       </c>
       <c r="K94" s="1">
@@ -5338,7 +5390,7 @@
         <v>76</v>
       </c>
       <c r="J95" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="K95" s="1">
@@ -5383,7 +5435,7 @@
         <v>214</v>
       </c>
       <c r="J96" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>260</v>
       </c>
       <c r="K96" s="1">
@@ -5428,7 +5480,7 @@
         <v>47</v>
       </c>
       <c r="J97" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>198</v>
       </c>
       <c r="K97" s="1">
@@ -5473,7 +5525,7 @@
         <v>5</v>
       </c>
       <c r="J98" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="K98" s="1">
@@ -5518,7 +5570,7 @@
         <v>16</v>
       </c>
       <c r="J99" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="K99" s="1">
@@ -5563,7 +5615,7 @@
         <v>232</v>
       </c>
       <c r="J100" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>374</v>
       </c>
       <c r="K100" s="1">
@@ -5608,7 +5660,7 @@
         <v>0</v>
       </c>
       <c r="J101" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="K101" s="1">
@@ -5653,7 +5705,7 @@
         <v>17</v>
       </c>
       <c r="J102" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="K102" s="1">
@@ -5698,7 +5750,7 @@
         <v>31</v>
       </c>
       <c r="J103" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="K103" s="1">
@@ -5743,7 +5795,7 @@
         <v>0</v>
       </c>
       <c r="J104" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="K104" s="1">
@@ -5788,7 +5840,7 @@
         <v>14</v>
       </c>
       <c r="J105" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="K105" s="1">
@@ -5833,7 +5885,7 @@
         <v>41</v>
       </c>
       <c r="J106" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>165</v>
       </c>
       <c r="K106" s="1">
@@ -5878,7 +5930,7 @@
         <v>0</v>
       </c>
       <c r="J107" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="K107" s="1">
@@ -5923,7 +5975,7 @@
         <v>12</v>
       </c>
       <c r="J108" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="K108" s="1">
@@ -5968,7 +6020,7 @@
         <v>4</v>
       </c>
       <c r="J109" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="K109" s="1">
@@ -6013,7 +6065,7 @@
         <v>52</v>
       </c>
       <c r="J110" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>151</v>
       </c>
       <c r="K110" s="1">
@@ -6058,7 +6110,7 @@
         <v>3</v>
       </c>
       <c r="J111" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="K111" s="1">
@@ -6103,7 +6155,7 @@
         <v>0</v>
       </c>
       <c r="J112" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K112" s="1">
@@ -6148,7 +6200,7 @@
         <v>1</v>
       </c>
       <c r="J113" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="K113" s="1">
@@ -6193,7 +6245,7 @@
         <v>0</v>
       </c>
       <c r="J114" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K114" s="1">
@@ -6238,7 +6290,7 @@
         <v>0</v>
       </c>
       <c r="J115" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="K115" s="1">
@@ -6283,7 +6335,7 @@
         <v>738</v>
       </c>
       <c r="J116" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1001</v>
       </c>
       <c r="K116" s="1">
@@ -6328,7 +6380,7 @@
         <v>24</v>
       </c>
       <c r="J117" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="K117" s="1">
@@ -6373,7 +6425,7 @@
         <v>720</v>
       </c>
       <c r="J118" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>931</v>
       </c>
       <c r="K118" s="1">
@@ -6418,7 +6470,7 @@
         <v>0</v>
       </c>
       <c r="J119" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="K119" s="1">
@@ -6463,7 +6515,7 @@
         <v>10</v>
       </c>
       <c r="J120" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="K120" s="1">
@@ -6508,7 +6560,7 @@
         <v>4</v>
       </c>
       <c r="J121" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="K121" s="1">
@@ -6553,7 +6605,7 @@
         <v>0</v>
       </c>
       <c r="J122" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="K122" s="1">
@@ -6598,7 +6650,7 @@
         <v>0</v>
       </c>
       <c r="J123" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="K123" s="1">
@@ -6643,7 +6695,7 @@
         <v>90</v>
       </c>
       <c r="J124" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>127</v>
       </c>
       <c r="K124" s="1">
@@ -6688,7 +6740,7 @@
         <v>404</v>
       </c>
       <c r="J125" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>742</v>
       </c>
       <c r="K125" s="1">
@@ -6733,7 +6785,7 @@
         <v>4</v>
       </c>
       <c r="J126" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="K126" s="1">
@@ -6778,7 +6830,7 @@
         <v>2</v>
       </c>
       <c r="J127" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="K127" s="1">
@@ -6823,7 +6875,7 @@
         <v>0</v>
       </c>
       <c r="J128" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="K128" s="1">
@@ -6868,7 +6920,7 @@
         <v>0</v>
       </c>
       <c r="J129" s="2">
-        <f t="shared" ref="J129:J191" si="2">SUM(F129:I129)</f>
+        <f t="shared" ref="J129:J191" si="3">SUM(F129:I129)</f>
         <v>38</v>
       </c>
       <c r="K129" s="1">
@@ -6913,7 +6965,7 @@
         <v>2</v>
       </c>
       <c r="J130" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="K130" s="1">
@@ -6958,7 +7010,7 @@
         <v>36</v>
       </c>
       <c r="J131" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="K131" s="1">
@@ -7003,7 +7055,7 @@
         <v>113</v>
       </c>
       <c r="J132" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>225</v>
       </c>
       <c r="K132" s="1">
@@ -7048,7 +7100,7 @@
         <v>61</v>
       </c>
       <c r="J133" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>212</v>
       </c>
       <c r="K133" s="1">
@@ -7093,7 +7145,7 @@
         <v>27</v>
       </c>
       <c r="J134" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="K134" s="1">
@@ -7138,7 +7190,7 @@
         <v>17</v>
       </c>
       <c r="J135" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>89</v>
       </c>
       <c r="K135" s="1">
@@ -7183,7 +7235,7 @@
         <v>0</v>
       </c>
       <c r="J136" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="K136" s="1">
@@ -7228,7 +7280,7 @@
         <v>323</v>
       </c>
       <c r="J137" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>385</v>
       </c>
       <c r="K137" s="1">
@@ -7273,7 +7325,7 @@
         <v>21</v>
       </c>
       <c r="J138" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>133</v>
       </c>
       <c r="K138" s="1">
@@ -7318,7 +7370,7 @@
         <v>46</v>
       </c>
       <c r="J139" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="K139" s="1">
@@ -7363,7 +7415,7 @@
         <v>3</v>
       </c>
       <c r="J140" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="K140" s="1">
@@ -7408,7 +7460,7 @@
         <v>196</v>
       </c>
       <c r="J141" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>321</v>
       </c>
       <c r="K141" s="1">
@@ -7453,7 +7505,7 @@
         <v>5</v>
       </c>
       <c r="J142" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="K142" s="1">
@@ -7498,7 +7550,7 @@
         <v>10</v>
       </c>
       <c r="J143" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="K143" s="1">
@@ -7543,7 +7595,7 @@
         <v>6</v>
       </c>
       <c r="J144" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
       <c r="K144" s="1">
@@ -7588,7 +7640,7 @@
         <v>12</v>
       </c>
       <c r="J145" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>113</v>
       </c>
       <c r="K145" s="1">
@@ -7633,7 +7685,7 @@
         <v>4</v>
       </c>
       <c r="J146" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="K146" s="1">
@@ -7678,7 +7730,7 @@
         <v>208</v>
       </c>
       <c r="J147" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>302</v>
       </c>
       <c r="K147" s="1">
@@ -7723,7 +7775,7 @@
         <v>153</v>
       </c>
       <c r="J148" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>293</v>
       </c>
       <c r="K148" s="1">
@@ -7768,7 +7820,7 @@
         <v>19</v>
       </c>
       <c r="J149" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="K149" s="1">
@@ -7813,7 +7865,7 @@
         <v>326</v>
       </c>
       <c r="J150" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>547</v>
       </c>
       <c r="K150" s="1">
@@ -7858,7 +7910,7 @@
         <v>239</v>
       </c>
       <c r="J151" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>462</v>
       </c>
       <c r="K151" s="1">
@@ -7903,7 +7955,7 @@
         <v>11</v>
       </c>
       <c r="J152" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="K152" s="1">
@@ -7948,7 +8000,7 @@
         <v>88</v>
       </c>
       <c r="J153" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>177</v>
       </c>
       <c r="K153" s="1">
@@ -7993,7 +8045,7 @@
         <v>57</v>
       </c>
       <c r="J154" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="K154" s="1">
@@ -8038,7 +8090,7 @@
         <v>0</v>
       </c>
       <c r="J155" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="K155" s="1">
@@ -8083,7 +8135,7 @@
         <v>5</v>
       </c>
       <c r="J156" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="K156" s="1">
@@ -8128,7 +8180,7 @@
         <v>56</v>
       </c>
       <c r="J157" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>183</v>
       </c>
       <c r="K157" s="1">
@@ -8173,7 +8225,7 @@
         <v>41</v>
       </c>
       <c r="J158" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>89</v>
       </c>
       <c r="K158" s="1">
@@ -8218,7 +8270,7 @@
         <v>2</v>
       </c>
       <c r="J159" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="K159" s="1">
@@ -8263,7 +8315,7 @@
         <v>0</v>
       </c>
       <c r="J160" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K160" s="1">
@@ -8308,7 +8360,7 @@
         <v>37</v>
       </c>
       <c r="J161" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="K161" s="1">
@@ -8353,7 +8405,7 @@
         <v>4</v>
       </c>
       <c r="J162" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="K162" s="1">
@@ -8398,7 +8450,7 @@
         <v>13</v>
       </c>
       <c r="J163" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
       <c r="K163" s="1">
@@ -8443,7 +8495,7 @@
         <v>5</v>
       </c>
       <c r="J164" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="K164" s="1">
@@ -8488,7 +8540,7 @@
         <v>62</v>
       </c>
       <c r="J165" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="K165" s="1">
@@ -8533,7 +8585,7 @@
         <v>68</v>
       </c>
       <c r="J166" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
       <c r="K166" s="1">
@@ -8578,7 +8630,7 @@
         <v>57</v>
       </c>
       <c r="J167" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="K167" s="1">
@@ -8623,7 +8675,7 @@
         <v>24</v>
       </c>
       <c r="J168" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="K168" s="1">
@@ -8668,7 +8720,7 @@
         <v>7</v>
       </c>
       <c r="J169" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="K169" s="1">
@@ -8713,7 +8765,7 @@
         <v>17</v>
       </c>
       <c r="J170" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
       <c r="K170" s="1">
@@ -8758,7 +8810,7 @@
         <v>46</v>
       </c>
       <c r="J171" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108</v>
       </c>
       <c r="K171" s="1">
@@ -8803,7 +8855,7 @@
         <v>147</v>
       </c>
       <c r="J172" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>332</v>
       </c>
       <c r="K172" s="1">
@@ -8848,7 +8900,7 @@
         <v>15</v>
       </c>
       <c r="J173" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="K173" s="1">
@@ -8893,7 +8945,7 @@
         <v>219</v>
       </c>
       <c r="J174" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>331</v>
       </c>
       <c r="K174" s="1">
@@ -8938,7 +8990,7 @@
         <v>290</v>
       </c>
       <c r="J175" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>390</v>
       </c>
       <c r="K175" s="1">
@@ -8983,7 +9035,7 @@
         <v>2</v>
       </c>
       <c r="J176" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="K176" s="1">
@@ -9028,7 +9080,7 @@
         <v>6</v>
       </c>
       <c r="J177" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="K177" s="1">
@@ -9073,7 +9125,7 @@
         <v>3</v>
       </c>
       <c r="J178" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="K178" s="1" t="s">
@@ -9118,7 +9170,7 @@
         <v>5</v>
       </c>
       <c r="J179" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="K179" s="1">
@@ -9163,7 +9215,7 @@
         <v>17</v>
       </c>
       <c r="J180" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="K180" s="1">
@@ -9208,7 +9260,7 @@
         <v>27</v>
       </c>
       <c r="J181" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
       <c r="K181" s="1">
@@ -9253,7 +9305,7 @@
         <v>11</v>
       </c>
       <c r="J182" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="K182" s="1">
@@ -9298,7 +9350,7 @@
         <v>4</v>
       </c>
       <c r="J183" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="K183" s="1">
@@ -9343,7 +9395,7 @@
         <v>4</v>
       </c>
       <c r="J184" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="K184" s="1">
@@ -9388,7 +9440,7 @@
         <v>18</v>
       </c>
       <c r="J185" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101</v>
       </c>
       <c r="K185" s="1">
@@ -9433,7 +9485,7 @@
         <v>12</v>
       </c>
       <c r="J186" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="K186" s="1">
@@ -9478,7 +9530,7 @@
         <v>629</v>
       </c>
       <c r="J187" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>890</v>
       </c>
       <c r="K187" s="1">
@@ -9523,7 +9575,7 @@
         <v>152</v>
       </c>
       <c r="J188" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>370</v>
       </c>
       <c r="K188" s="1">
@@ -9568,7 +9620,7 @@
         <v>1</v>
       </c>
       <c r="J189" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="K189" s="1">
@@ -9613,7 +9665,7 @@
         <v>12</v>
       </c>
       <c r="J190" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="K190" s="1">
@@ -9658,7 +9710,7 @@
         <v>4</v>
       </c>
       <c r="J191" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="K191" s="1">
@@ -9703,7 +9755,7 @@
         <v>2</v>
       </c>
       <c r="J192" s="2">
-        <f t="shared" ref="J192:J212" si="3">SUM(F192:I192)</f>
+        <f t="shared" ref="J192:J212" si="4">SUM(F192:I192)</f>
         <v>44</v>
       </c>
       <c r="K192" s="1">
@@ -9748,7 +9800,7 @@
         <v>7</v>
       </c>
       <c r="J193" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="K193" s="1">
@@ -9793,7 +9845,7 @@
         <v>107</v>
       </c>
       <c r="J194" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>277</v>
       </c>
       <c r="K194" s="1">
@@ -9838,7 +9890,7 @@
         <v>4</v>
       </c>
       <c r="J195" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="K195" s="1">
@@ -9883,7 +9935,7 @@
         <v>9</v>
       </c>
       <c r="J196" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="K196" s="1">
@@ -9928,7 +9980,7 @@
         <v>0</v>
       </c>
       <c r="J197" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="K197" s="1">
@@ -9973,7 +10025,7 @@
         <v>64</v>
       </c>
       <c r="J198" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>180</v>
       </c>
       <c r="K198" s="1">
@@ -10018,7 +10070,7 @@
         <v>19</v>
       </c>
       <c r="J199" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="K199" s="1">
@@ -10063,7 +10115,7 @@
         <v>0</v>
       </c>
       <c r="J200" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="K200" s="1">
@@ -10108,7 +10160,7 @@
         <v>41</v>
       </c>
       <c r="J201" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>102</v>
       </c>
       <c r="K201" s="1">
@@ -10153,7 +10205,7 @@
         <v>474</v>
       </c>
       <c r="J202" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>838</v>
       </c>
       <c r="K202" s="1">
@@ -10198,7 +10250,7 @@
         <v>22</v>
       </c>
       <c r="J203" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>95</v>
       </c>
       <c r="K203" s="1">
@@ -10243,7 +10295,7 @@
         <v>17</v>
       </c>
       <c r="J204" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="K204" s="1">
@@ -10288,7 +10340,7 @@
         <v>10</v>
       </c>
       <c r="J205" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="K205" s="1">
@@ -10333,7 +10385,7 @@
         <v>82</v>
       </c>
       <c r="J206" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>210</v>
       </c>
       <c r="K206" s="1">
@@ -10378,7 +10430,7 @@
         <v>205</v>
       </c>
       <c r="J207" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>387</v>
       </c>
       <c r="K207" s="1">
@@ -10423,7 +10475,7 @@
         <v>12</v>
       </c>
       <c r="J208" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="K208" s="1">
@@ -10468,7 +10520,7 @@
         <v>3</v>
       </c>
       <c r="J209" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="K209" s="1" t="s">
@@ -10513,7 +10565,7 @@
         <v>163</v>
       </c>
       <c r="J210" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
       <c r="K210" s="1">
@@ -10558,7 +10610,7 @@
         <v>21</v>
       </c>
       <c r="J211" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="K211" s="1">
@@ -10603,7 +10655,7 @@
         <v>43</v>
       </c>
       <c r="J212" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="K212" s="1">

</xml_diff>

<commit_message>
Add conclusion, fix scatterplot, rename index page
</commit_message>
<xml_diff>
--- a/Archive folder/data_cleanup/deforestation_cleanup.xlsx
+++ b/Archive folder/data_cleanup/deforestation_cleanup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="239">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -721,6 +721,18 @@
   </si>
   <si>
     <t>pM delta</t>
+  </si>
+  <si>
+    <t>fA delta (total sq. km)</t>
+  </si>
+  <si>
+    <t>df delta (avg %)</t>
+  </si>
+  <si>
+    <t>pL delta  (avg %)</t>
+  </si>
+  <si>
+    <t>pM delta (avg %)</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1121,7 @@
   <dimension ref="A1:U212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,6 +1376,18 @@
       <c r="N5" s="1">
         <v>17.3</v>
       </c>
+      <c r="P5" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>236</v>
+      </c>
+      <c r="R5" t="s">
+        <v>237</v>
+      </c>
+      <c r="S5" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1408,6 +1432,22 @@
       </c>
       <c r="N6" s="1">
         <v>0</v>
+      </c>
+      <c r="P6">
+        <f>SUM(C2:C212)-SUM(B2:B212)</f>
+        <v>-1305</v>
+      </c>
+      <c r="Q6">
+        <f>AVERAGE(E2:E212)-AVERAGE(D2:D212)</f>
+        <v>9.2975609756097588E-2</v>
+      </c>
+      <c r="R6">
+        <f>AVERAGE(L2:L212)-AVERAGE(K2:K212)</f>
+        <v>7.6125603864734366</v>
+      </c>
+      <c r="S6">
+        <f>AVERAGE(N2:N212)-AVERAGE(M2:M212)</f>
+        <v>6.9439613526570048</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -10699,7 +10739,7 @@
   <dimension ref="B1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10757,7 +10797,7 @@
   <dimension ref="A1:P212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10818,11 +10858,11 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <f>D2-C2</f>
+        <f t="shared" ref="I2:I65" si="0">D2-C2</f>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="J2">
-        <f>F2-E2</f>
+        <f t="shared" ref="J2:J65" si="1">F2-E2</f>
         <v>0</v>
       </c>
       <c r="L2" s="2">
@@ -10833,11 +10873,11 @@
         <v>-8.4003949359543445E-2</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:P2" si="0">CORREL(I2:I212,$L2:$L212)</f>
+        <f t="shared" ref="O2:P2" si="2">CORREL(I2:I212,$L2:$L212)</f>
         <v>-2.301266362357697E-2</v>
       </c>
       <c r="P2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.1030750598764379E-2</v>
       </c>
     </row>
@@ -10861,15 +10901,15 @@
         <v>1.5</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H66" si="1">B3-A3</f>
+        <f t="shared" ref="H3:H66" si="3">B3-A3</f>
         <v>-0.27</v>
       </c>
       <c r="I3">
-        <f>D3-C3</f>
+        <f t="shared" si="0"/>
         <v>2.0999999999999996</v>
       </c>
       <c r="J3">
-        <f>F3-E3</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="L3" s="2">
@@ -10896,15 +10936,15 @@
         <v>1.2</v>
       </c>
       <c r="H4">
+        <f t="shared" si="3"/>
+        <v>-1.98</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>1.6000000000000005</v>
+      </c>
+      <c r="J4">
         <f t="shared" si="1"/>
-        <v>-1.98</v>
-      </c>
-      <c r="I4">
-        <f>D4-C4</f>
-        <v>1.6000000000000005</v>
-      </c>
-      <c r="J4">
-        <f>F4-E4</f>
         <v>1.0999999999999999</v>
       </c>
       <c r="L4" s="2">
@@ -10931,15 +10971,15 @@
         <v>17.3</v>
       </c>
       <c r="H5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>1.1999999999999993</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <f>D5-C5</f>
-        <v>1.1999999999999993</v>
-      </c>
-      <c r="J5">
-        <f>F5-E5</f>
         <v>15</v>
       </c>
       <c r="L5" s="2">
@@ -10966,15 +11006,15 @@
         <v>0</v>
       </c>
       <c r="H6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <f>D6-C6</f>
-        <v>14</v>
-      </c>
-      <c r="J6">
-        <f>F6-E6</f>
         <v>0</v>
       </c>
       <c r="L6" s="2">
@@ -11001,15 +11041,15 @@
         <v>0.1</v>
       </c>
       <c r="H7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <f>D7-C7</f>
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <f>F7-E7</f>
         <v>0</v>
       </c>
       <c r="L7" s="2">
@@ -11036,15 +11076,15 @@
         <v>1.4</v>
       </c>
       <c r="H8">
+        <f t="shared" si="3"/>
+        <v>-0.16999999999999998</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="1"/>
-        <v>-0.16999999999999998</v>
-      </c>
-      <c r="I8">
-        <f>D8-C8</f>
-        <v>5.5</v>
-      </c>
-      <c r="J8">
-        <f>F8-E8</f>
         <v>1.2</v>
       </c>
       <c r="L8" s="2">
@@ -11071,15 +11111,15 @@
         <v>8.9</v>
       </c>
       <c r="H9">
+        <f t="shared" si="3"/>
+        <v>0.19000000000000006</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>2.3999999999999995</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="1"/>
-        <v>0.19000000000000006</v>
-      </c>
-      <c r="I9">
-        <f>D9-C9</f>
-        <v>2.3999999999999995</v>
-      </c>
-      <c r="J9">
-        <f>F9-E9</f>
         <v>6.2</v>
       </c>
       <c r="L9" s="2">
@@ -11106,15 +11146,15 @@
         <v>0</v>
       </c>
       <c r="H10">
+        <f t="shared" si="3"/>
+        <v>-3.9999999999999994E-2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="1"/>
-        <v>-3.9999999999999994E-2</v>
-      </c>
-      <c r="I10">
-        <f>D10-C10</f>
-        <v>16.899999999999999</v>
-      </c>
-      <c r="J10">
-        <f>F10-E10</f>
         <v>0</v>
       </c>
       <c r="L10" s="2">
@@ -11141,15 +11181,15 @@
         <v>0</v>
       </c>
       <c r="H11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f>D11-C11</f>
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <f>F11-E11</f>
         <v>0</v>
       </c>
       <c r="L11" s="2">
@@ -11176,15 +11216,15 @@
         <v>48.5</v>
       </c>
       <c r="H12">
+        <f t="shared" si="3"/>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="1"/>
-        <v>0.22999999999999998</v>
-      </c>
-      <c r="I12">
-        <f>D12-C12</f>
-        <v>7</v>
-      </c>
-      <c r="J12">
-        <f>F12-E12</f>
         <v>21.9</v>
       </c>
       <c r="L12" s="2">
@@ -11211,15 +11251,15 @@
         <v>0</v>
       </c>
       <c r="H13">
+        <f t="shared" si="3"/>
+        <v>0.11</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J13">
         <f t="shared" si="1"/>
-        <v>0.11</v>
-      </c>
-      <c r="I13">
-        <f>D13-C13</f>
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="J13">
-        <f>F13-E13</f>
         <v>0</v>
       </c>
       <c r="L13" s="2">
@@ -11246,15 +11286,15 @@
         <v>0</v>
       </c>
       <c r="H14">
+        <f t="shared" si="3"/>
+        <v>-1.57</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J14">
         <f t="shared" si="1"/>
-        <v>-1.57</v>
-      </c>
-      <c r="I14">
-        <f>D14-C14</f>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="J14">
-        <f>F14-E14</f>
         <v>0</v>
       </c>
       <c r="L14" s="2">
@@ -11281,15 +11321,15 @@
         <v>0.4</v>
       </c>
       <c r="H15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000011</v>
+      </c>
+      <c r="J15">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <f>D15-C15</f>
-        <v>7.2000000000000011</v>
-      </c>
-      <c r="J15">
-        <f>F15-E15</f>
         <v>0.2</v>
       </c>
       <c r="L15" s="2">
@@ -11316,15 +11356,15 @@
         <v>7.6</v>
       </c>
       <c r="H16">
+        <f t="shared" si="3"/>
+        <v>2.06</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="J16">
         <f t="shared" si="1"/>
-        <v>2.06</v>
-      </c>
-      <c r="I16">
-        <f>D16-C16</f>
-        <v>1.5</v>
-      </c>
-      <c r="J16">
-        <f>F16-E16</f>
         <v>7.6</v>
       </c>
       <c r="L16" s="2">
@@ -11351,15 +11391,15 @@
         <v>2.5</v>
       </c>
       <c r="H17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>3.8</v>
+      </c>
+      <c r="J17">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <f>D17-C17</f>
-        <v>3.8</v>
-      </c>
-      <c r="J17">
-        <f>F17-E17</f>
         <v>2.4</v>
       </c>
       <c r="L17" s="2">
@@ -11386,15 +11426,15 @@
         <v>0.1</v>
       </c>
       <c r="H18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="J18">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <f>D18-C18</f>
-        <v>0.1</v>
-      </c>
-      <c r="J18">
-        <f>F18-E18</f>
         <v>0</v>
       </c>
       <c r="L18" s="2">
@@ -11421,15 +11461,15 @@
         <v>0</v>
       </c>
       <c r="H19">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="J19">
         <f t="shared" si="1"/>
-        <v>0.33999999999999997</v>
-      </c>
-      <c r="I19">
-        <f>D19-C19</f>
-        <v>2.0999999999999996</v>
-      </c>
-      <c r="J19">
-        <f>F19-E19</f>
         <v>0</v>
       </c>
       <c r="L19" s="2">
@@ -11456,15 +11496,15 @@
         <v>56.1</v>
       </c>
       <c r="H20">
+        <f t="shared" si="3"/>
+        <v>-0.16</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>15.799999999999999</v>
+      </c>
+      <c r="J20">
         <f t="shared" si="1"/>
-        <v>-0.16</v>
-      </c>
-      <c r="I20">
-        <f>D20-C20</f>
-        <v>15.799999999999999</v>
-      </c>
-      <c r="J20">
-        <f>F20-E20</f>
         <v>52.4</v>
       </c>
       <c r="L20" s="2">
@@ -11491,15 +11531,15 @@
         <v>14.2</v>
       </c>
       <c r="H21">
+        <f t="shared" si="3"/>
+        <v>-0.57000000000000006</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>10.700000000000003</v>
+      </c>
+      <c r="J21">
         <f t="shared" si="1"/>
-        <v>-0.57000000000000006</v>
-      </c>
-      <c r="I21">
-        <f>D21-C21</f>
-        <v>10.700000000000003</v>
-      </c>
-      <c r="J21">
-        <f>F21-E21</f>
         <v>13.7</v>
       </c>
       <c r="L21" s="2">
@@ -11526,15 +11566,15 @@
         <v>0</v>
       </c>
       <c r="H22">
+        <f t="shared" si="3"/>
+        <v>-0.22999999999999998</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000007</v>
+      </c>
+      <c r="J22">
         <f t="shared" si="1"/>
-        <v>-0.22999999999999998</v>
-      </c>
-      <c r="I22">
-        <f>D22-C22</f>
-        <v>4.3000000000000007</v>
-      </c>
-      <c r="J22">
-        <f>F22-E22</f>
         <v>0</v>
       </c>
       <c r="L22" s="2">
@@ -11561,15 +11601,15 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="H23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999947</v>
+      </c>
+      <c r="J23">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <f>D23-C23</f>
-        <v>0.39999999999999947</v>
-      </c>
-      <c r="J23">
-        <f>F23-E23</f>
         <v>0.29999999999999982</v>
       </c>
       <c r="L23" s="2">
@@ -11596,15 +11636,15 @@
         <v>0</v>
       </c>
       <c r="H24">
+        <f t="shared" si="3"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>33.099999999999994</v>
+      </c>
+      <c r="J24">
         <f t="shared" si="1"/>
-        <v>2.0000000000000018E-2</v>
-      </c>
-      <c r="I24">
-        <f>D24-C24</f>
-        <v>33.099999999999994</v>
-      </c>
-      <c r="J24">
-        <f>F24-E24</f>
         <v>0</v>
       </c>
       <c r="L24" s="2">
@@ -11631,15 +11671,15 @@
         <v>0</v>
       </c>
       <c r="H25">
+        <f t="shared" si="3"/>
+        <v>0.18</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="1"/>
-        <v>0.18</v>
-      </c>
-      <c r="I25">
-        <f>D25-C25</f>
-        <v>16</v>
-      </c>
-      <c r="J25">
-        <f>F25-E25</f>
         <v>0</v>
       </c>
       <c r="L25" s="2">
@@ -11666,15 +11706,15 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="H26">
+        <f t="shared" si="3"/>
+        <v>-0.11</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+      <c r="J26">
         <f t="shared" si="1"/>
-        <v>-0.11</v>
-      </c>
-      <c r="I26">
-        <f>D26-C26</f>
-        <v>1.3</v>
-      </c>
-      <c r="J26">
-        <f>F26-E26</f>
         <v>1.2000000000000011</v>
       </c>
       <c r="L26" s="2">
@@ -11701,15 +11741,15 @@
         <v>0</v>
       </c>
       <c r="H27">
+        <f t="shared" si="3"/>
+        <v>5.9999999999999942E-2</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>11.3</v>
+      </c>
+      <c r="J27">
         <f t="shared" si="1"/>
-        <v>5.9999999999999942E-2</v>
-      </c>
-      <c r="I27">
-        <f>D27-C27</f>
-        <v>11.3</v>
-      </c>
-      <c r="J27">
-        <f>F27-E27</f>
         <v>0</v>
       </c>
       <c r="L27" s="2">
@@ -11736,15 +11776,15 @@
         <v>20.5</v>
       </c>
       <c r="H28">
+        <f t="shared" si="3"/>
+        <v>-0.12</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>21.7</v>
+      </c>
+      <c r="J28">
         <f t="shared" si="1"/>
-        <v>-0.12</v>
-      </c>
-      <c r="I28">
-        <f>D28-C28</f>
-        <v>21.7</v>
-      </c>
-      <c r="J28">
-        <f>F28-E28</f>
         <v>18</v>
       </c>
       <c r="L28" s="2">
@@ -11771,15 +11811,15 @@
         <v>1.5</v>
       </c>
       <c r="H29">
+        <f t="shared" si="3"/>
+        <v>-0.10000000000000003</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000028</v>
+      </c>
+      <c r="J29">
         <f t="shared" si="1"/>
-        <v>-0.10000000000000003</v>
-      </c>
-      <c r="I29">
-        <f>D29-C29</f>
-        <v>7.2000000000000028</v>
-      </c>
-      <c r="J29">
-        <f>F29-E29</f>
         <v>0</v>
       </c>
       <c r="L29" s="2">
@@ -11806,15 +11846,15 @@
         <v>15.3</v>
       </c>
       <c r="H30">
+        <f t="shared" si="3"/>
+        <v>-0.69</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>38.5</v>
+      </c>
+      <c r="J30">
         <f t="shared" si="1"/>
-        <v>-0.69</v>
-      </c>
-      <c r="I30">
-        <f>D30-C30</f>
-        <v>38.5</v>
-      </c>
-      <c r="J30">
-        <f>F30-E30</f>
         <v>15.200000000000001</v>
       </c>
       <c r="L30" s="2">
@@ -11841,15 +11881,15 @@
         <v>0</v>
       </c>
       <c r="H31">
+        <f t="shared" si="3"/>
+        <v>0.12</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="J31">
         <f t="shared" si="1"/>
-        <v>0.12</v>
-      </c>
-      <c r="I31">
-        <f>D31-C31</f>
-        <v>1.5</v>
-      </c>
-      <c r="J31">
-        <f>F31-E31</f>
         <v>0</v>
       </c>
       <c r="L31" s="2">
@@ -11876,15 +11916,15 @@
         <v>0</v>
       </c>
       <c r="H32">
+        <f t="shared" si="3"/>
+        <v>-5.95</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>3.1000000000000005</v>
+      </c>
+      <c r="J32">
         <f t="shared" si="1"/>
-        <v>-5.95</v>
-      </c>
-      <c r="I32">
-        <f>D32-C32</f>
-        <v>3.1000000000000005</v>
-      </c>
-      <c r="J32">
-        <f>F32-E32</f>
         <v>0</v>
       </c>
       <c r="L32" s="2">
@@ -11911,15 +11951,15 @@
         <v>0</v>
       </c>
       <c r="H33">
+        <f t="shared" si="3"/>
+        <v>2.97</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="J33">
         <f t="shared" si="1"/>
-        <v>2.97</v>
-      </c>
-      <c r="I33">
-        <f>D33-C33</f>
-        <v>0.10000000000000009</v>
-      </c>
-      <c r="J33">
-        <f>F33-E33</f>
         <v>0</v>
       </c>
       <c r="L33" s="2">
@@ -11946,15 +11986,15 @@
         <v>0.5</v>
       </c>
       <c r="H34">
+        <f t="shared" si="3"/>
+        <v>0.18000000000000016</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="J34">
         <f t="shared" si="1"/>
-        <v>0.18000000000000016</v>
-      </c>
-      <c r="I34">
-        <f>D34-C34</f>
-        <v>26</v>
-      </c>
-      <c r="J34">
-        <f>F34-E34</f>
         <v>0.5</v>
       </c>
       <c r="L34" s="2">
@@ -11981,15 +12021,15 @@
         <v>6.8</v>
       </c>
       <c r="H35">
+        <f t="shared" si="3"/>
+        <v>0.13000000000000012</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J35">
         <f t="shared" si="1"/>
-        <v>0.13000000000000012</v>
-      </c>
-      <c r="I35">
-        <f>D35-C35</f>
-        <v>5</v>
-      </c>
-      <c r="J35">
-        <f>F35-E35</f>
         <v>6.2</v>
       </c>
       <c r="L35" s="2">
@@ -12016,15 +12056,15 @@
         <v>1.4</v>
       </c>
       <c r="H36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>3.6000000000000005</v>
+      </c>
+      <c r="J36">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <f>D36-C36</f>
-        <v>3.6000000000000005</v>
-      </c>
-      <c r="J36">
-        <f>F36-E36</f>
         <v>0.7</v>
       </c>
       <c r="L36" s="2">
@@ -12051,15 +12091,15 @@
         <v>1.2</v>
       </c>
       <c r="H37">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999996</v>
+      </c>
+      <c r="J37">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <f>D37-C37</f>
-        <v>1.5999999999999996</v>
-      </c>
-      <c r="J37">
-        <f>F37-E37</f>
         <v>9.9999999999999867E-2</v>
       </c>
       <c r="L37" s="2">
@@ -12086,15 +12126,15 @@
         <v>0</v>
       </c>
       <c r="H38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>0.40000000000000213</v>
+      </c>
+      <c r="J38">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <f>D38-C38</f>
-        <v>0.40000000000000213</v>
-      </c>
-      <c r="J38">
-        <f>F38-E38</f>
         <v>0</v>
       </c>
       <c r="L38" s="2">
@@ -12121,15 +12161,15 @@
         <v>0</v>
       </c>
       <c r="H39">
+        <f t="shared" si="3"/>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>6.1000000000000014</v>
+      </c>
+      <c r="J39">
         <f t="shared" si="1"/>
-        <v>1.1400000000000001</v>
-      </c>
-      <c r="I39">
-        <f>D39-C39</f>
-        <v>6.1000000000000014</v>
-      </c>
-      <c r="J39">
-        <f>F39-E39</f>
         <v>0</v>
       </c>
       <c r="L39" s="2">
@@ -12156,15 +12196,15 @@
         <v>0</v>
       </c>
       <c r="H40">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J40">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <f>D40-C40</f>
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <f>F40-E40</f>
         <v>0</v>
       </c>
       <c r="L40" s="2">
@@ -12191,15 +12231,15 @@
         <v>3.9</v>
       </c>
       <c r="H41">
+        <f t="shared" si="3"/>
+        <v>-0.39</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999993</v>
+      </c>
+      <c r="J41">
         <f t="shared" si="1"/>
-        <v>-0.39</v>
-      </c>
-      <c r="I41">
-        <f>D41-C41</f>
-        <v>2.1999999999999993</v>
-      </c>
-      <c r="J41">
-        <f>F41-E41</f>
         <v>0.60000000000000009</v>
       </c>
       <c r="L41" s="2">
@@ -12226,15 +12266,15 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="H42">
+        <f t="shared" si="3"/>
+        <v>0.10999999999999988</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="J42">
         <f t="shared" si="1"/>
-        <v>0.10999999999999988</v>
-      </c>
-      <c r="I42">
-        <f>D42-C42</f>
-        <v>3.4000000000000004</v>
-      </c>
-      <c r="J42">
-        <f>F42-E42</f>
         <v>1.9</v>
       </c>
       <c r="L42" s="2">
@@ -12261,15 +12301,15 @@
         <v>0</v>
       </c>
       <c r="H43">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>0.69999999999999574</v>
+      </c>
+      <c r="J43">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <f>D43-C43</f>
-        <v>0.69999999999999574</v>
-      </c>
-      <c r="J43">
-        <f>F43-E43</f>
         <v>0</v>
       </c>
       <c r="L43" s="2">
@@ -12296,15 +12336,15 @@
         <v>0</v>
       </c>
       <c r="H44">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J44">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <f>D44-C44</f>
-        <v>0</v>
-      </c>
-      <c r="J44">
-        <f>F44-E44</f>
         <v>0</v>
       </c>
       <c r="L44" s="2">
@@ -12331,15 +12371,15 @@
         <v>16.899999999999999</v>
       </c>
       <c r="H45">
+        <f t="shared" si="3"/>
+        <v>-4.9999999999999989E-2</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>3.6000000000000014</v>
+      </c>
+      <c r="J45">
         <f t="shared" si="1"/>
-        <v>-4.9999999999999989E-2</v>
-      </c>
-      <c r="I45">
-        <f>D45-C45</f>
-        <v>3.6000000000000014</v>
-      </c>
-      <c r="J45">
-        <f>F45-E45</f>
         <v>14.499999999999998</v>
       </c>
       <c r="L45" s="2">
@@ -12366,15 +12406,15 @@
         <v>0.3</v>
       </c>
       <c r="H46">
+        <f t="shared" si="3"/>
+        <v>0.45000000000000007</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="0"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J46">
         <f t="shared" si="1"/>
-        <v>0.45000000000000007</v>
-      </c>
-      <c r="I46">
-        <f>D46-C46</f>
-        <v>10.199999999999999</v>
-      </c>
-      <c r="J46">
-        <f>F46-E46</f>
         <v>0.3</v>
       </c>
       <c r="L46" s="2">
@@ -12401,15 +12441,15 @@
         <v>4.3</v>
       </c>
       <c r="H47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J47">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <f>D47-C47</f>
-        <v>2</v>
-      </c>
-      <c r="J47">
-        <f>F47-E47</f>
         <v>0.5</v>
       </c>
       <c r="L47" s="2">
@@ -12436,15 +12476,15 @@
         <v>33.6</v>
       </c>
       <c r="H48">
+        <f t="shared" si="3"/>
+        <v>-9.999999999999995E-3</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="0"/>
+        <v>33.5</v>
+      </c>
+      <c r="J48">
         <f t="shared" si="1"/>
-        <v>-9.999999999999995E-3</v>
-      </c>
-      <c r="I48">
-        <f>D48-C48</f>
-        <v>33.5</v>
-      </c>
-      <c r="J48">
-        <f>F48-E48</f>
         <v>33.6</v>
       </c>
       <c r="L48" s="2">
@@ -12471,15 +12511,15 @@
         <v>15.8</v>
       </c>
       <c r="H49">
+        <f t="shared" si="3"/>
+        <v>-1.75</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="J49">
         <f t="shared" si="1"/>
-        <v>-1.75</v>
-      </c>
-      <c r="I49">
-        <f>D49-C49</f>
-        <v>7.5</v>
-      </c>
-      <c r="J49">
-        <f>F49-E49</f>
         <v>3.9000000000000004</v>
       </c>
       <c r="L49" s="2">
@@ -12506,15 +12546,15 @@
         <v>2.1</v>
       </c>
       <c r="H50">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="0"/>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="J50">
         <f t="shared" si="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="I50">
-        <f>D50-C50</f>
-        <v>0.29999999999999716</v>
-      </c>
-      <c r="J50">
-        <f>F50-E50</f>
         <v>2</v>
       </c>
       <c r="L50" s="2">
@@ -12541,15 +12581,15 @@
         <v>16.3</v>
       </c>
       <c r="H51">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="0"/>
+        <v>30.000000000000004</v>
+      </c>
+      <c r="J51">
         <f t="shared" si="1"/>
-        <v>0.06</v>
-      </c>
-      <c r="I51">
-        <f>D51-C51</f>
-        <v>30.000000000000004</v>
-      </c>
-      <c r="J51">
-        <f>F51-E51</f>
         <v>14.9</v>
       </c>
       <c r="L51" s="2">
@@ -12576,15 +12616,15 @@
         <v>7.6</v>
       </c>
       <c r="H52">
+        <f t="shared" si="3"/>
+        <v>-0.14000000000000012</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="0"/>
+        <v>8.1000000000000014</v>
+      </c>
+      <c r="J52">
         <f t="shared" si="1"/>
-        <v>-0.14000000000000012</v>
-      </c>
-      <c r="I52">
-        <f>D52-C52</f>
-        <v>8.1000000000000014</v>
-      </c>
-      <c r="J52">
-        <f>F52-E52</f>
         <v>6.3</v>
       </c>
       <c r="L52" s="2">
@@ -12611,15 +12651,15 @@
         <v>0.9</v>
       </c>
       <c r="H53">
+        <f t="shared" si="3"/>
+        <v>0.59</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="0"/>
+        <v>17.899999999999999</v>
+      </c>
+      <c r="J53">
         <f t="shared" si="1"/>
-        <v>0.59</v>
-      </c>
-      <c r="I53">
-        <f>D53-C53</f>
-        <v>17.899999999999999</v>
-      </c>
-      <c r="J53">
-        <f>F53-E53</f>
         <v>0.9</v>
       </c>
       <c r="L53" s="2">
@@ -12646,15 +12686,15 @@
         <v>0</v>
       </c>
       <c r="H54">
+        <f t="shared" si="3"/>
+        <v>-0.05</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000018</v>
+      </c>
+      <c r="J54">
         <f t="shared" si="1"/>
-        <v>-0.05</v>
-      </c>
-      <c r="I54">
-        <f>D54-C54</f>
-        <v>8.0000000000000018</v>
-      </c>
-      <c r="J54">
-        <f>F54-E54</f>
         <v>0</v>
       </c>
       <c r="L54" s="2">
@@ -12681,15 +12721,15 @@
         <v>29.2</v>
       </c>
       <c r="H55">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="0"/>
+        <v>7.8000000000000007</v>
+      </c>
+      <c r="J55">
         <f t="shared" si="1"/>
-        <v>0.45</v>
-      </c>
-      <c r="I55">
-        <f>D55-C55</f>
-        <v>7.8000000000000007</v>
-      </c>
-      <c r="J55">
-        <f>F55-E55</f>
         <v>9.5</v>
       </c>
       <c r="L55" s="2">
@@ -12716,15 +12756,15 @@
         <v>0.2</v>
       </c>
       <c r="H56">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+      <c r="J56">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <f>D56-C56</f>
-        <v>1.3</v>
-      </c>
-      <c r="J56">
-        <f>F56-E56</f>
         <v>0.2</v>
       </c>
       <c r="L56" s="2">
@@ -12751,15 +12791,15 @@
         <v>0.1</v>
       </c>
       <c r="H57">
+        <f t="shared" si="3"/>
+        <v>3.9999999999999925E-2</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="0"/>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="J57">
         <f t="shared" si="1"/>
-        <v>3.9999999999999925E-2</v>
-      </c>
-      <c r="I57">
-        <f>D57-C57</f>
-        <v>0.10000000000000142</v>
-      </c>
-      <c r="J57">
-        <f>F57-E57</f>
         <v>0</v>
       </c>
       <c r="L57" s="2">
@@ -12786,15 +12826,15 @@
         <v>31.4</v>
       </c>
       <c r="H58">
+        <f t="shared" si="3"/>
+        <v>1.0699999999999998</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J58">
         <f t="shared" si="1"/>
-        <v>1.0699999999999998</v>
-      </c>
-      <c r="I58">
-        <f>D58-C58</f>
-        <v>3</v>
-      </c>
-      <c r="J58">
-        <f>F58-E58</f>
         <v>19.5</v>
       </c>
       <c r="L58" s="2">
@@ -12821,15 +12861,15 @@
         <v>75.7</v>
       </c>
       <c r="H59">
+        <f t="shared" si="3"/>
+        <v>-3.0000000000000027E-2</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="0"/>
+        <v>3.8000000000000007</v>
+      </c>
+      <c r="J59">
         <f t="shared" si="1"/>
-        <v>-3.0000000000000027E-2</v>
-      </c>
-      <c r="I59">
-        <f>D59-C59</f>
-        <v>3.8000000000000007</v>
-      </c>
-      <c r="J59">
-        <f>F59-E59</f>
         <v>1</v>
       </c>
       <c r="L59" s="2">
@@ -12856,15 +12896,15 @@
         <v>13.2</v>
       </c>
       <c r="H60">
+        <f t="shared" si="3"/>
+        <v>1.55</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="0"/>
+        <v>10.799999999999999</v>
+      </c>
+      <c r="J60">
         <f t="shared" si="1"/>
-        <v>1.55</v>
-      </c>
-      <c r="I60">
-        <f>D60-C60</f>
-        <v>10.799999999999999</v>
-      </c>
-      <c r="J60">
-        <f>F60-E60</f>
         <v>11.6</v>
       </c>
       <c r="L60" s="2">
@@ -12891,15 +12931,15 @@
         <v>9.5</v>
       </c>
       <c r="H61">
+        <f t="shared" si="3"/>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
+      </c>
+      <c r="J61">
         <f t="shared" si="1"/>
-        <v>0.22999999999999998</v>
-      </c>
-      <c r="I61">
-        <f>D61-C61</f>
-        <v>8.4</v>
-      </c>
-      <c r="J61">
-        <f>F61-E61</f>
         <v>9.5</v>
       </c>
       <c r="L61" s="2">
@@ -12926,15 +12966,15 @@
         <v>2.7</v>
       </c>
       <c r="H62">
+        <f t="shared" si="3"/>
+        <v>4.9999999999999933E-2</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="0"/>
+        <v>17.8</v>
+      </c>
+      <c r="J62">
         <f t="shared" si="1"/>
-        <v>4.9999999999999933E-2</v>
-      </c>
-      <c r="I62">
-        <f>D62-C62</f>
-        <v>17.8</v>
-      </c>
-      <c r="J62">
-        <f>F62-E62</f>
         <v>2.7</v>
       </c>
       <c r="L62" s="2">
@@ -12961,15 +13001,15 @@
         <v>0</v>
       </c>
       <c r="H63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999645E-2</v>
+      </c>
+      <c r="J63">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I63">
-        <f>D63-C63</f>
-        <v>9.9999999999999645E-2</v>
-      </c>
-      <c r="J63">
-        <f>F63-E63</f>
         <v>0</v>
       </c>
       <c r="L63" s="2">
@@ -12996,15 +13036,15 @@
         <v>27.5</v>
       </c>
       <c r="H64">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="0"/>
+        <v>19.599999999999998</v>
+      </c>
+      <c r="J64">
         <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="I64">
-        <f>D64-C64</f>
-        <v>19.599999999999998</v>
-      </c>
-      <c r="J64">
-        <f>F64-E64</f>
         <v>27.3</v>
       </c>
       <c r="L64" s="2">
@@ -13031,15 +13071,15 @@
         <v>0</v>
       </c>
       <c r="H65">
+        <f t="shared" si="3"/>
+        <v>-1.37</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="0"/>
+        <v>0.69999999999999929</v>
+      </c>
+      <c r="J65">
         <f t="shared" si="1"/>
-        <v>-1.37</v>
-      </c>
-      <c r="I65">
-        <f>D65-C65</f>
-        <v>0.69999999999999929</v>
-      </c>
-      <c r="J65">
-        <f>F65-E65</f>
         <v>0</v>
       </c>
       <c r="L65" s="2">
@@ -13066,15 +13106,15 @@
         <v>0</v>
       </c>
       <c r="H66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I66">
-        <f>D66-C66</f>
+        <f t="shared" ref="I66:I129" si="4">D66-C66</f>
         <v>0</v>
       </c>
       <c r="J66">
-        <f>F66-E66</f>
+        <f t="shared" ref="J66:J129" si="5">F66-E66</f>
         <v>0</v>
       </c>
       <c r="L66" s="2">
@@ -13101,15 +13141,15 @@
         <v>6.2</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H130" si="2">B67-A67</f>
+        <f t="shared" ref="H67:H130" si="6">B67-A67</f>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="I67">
-        <f>D67-C67</f>
+        <f t="shared" si="4"/>
         <v>3.2</v>
       </c>
       <c r="J67">
-        <f>F67-E67</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L67" s="2">
@@ -13136,15 +13176,15 @@
         <v>16.7</v>
       </c>
       <c r="H68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33</v>
       </c>
       <c r="I68">
-        <f>D68-C68</f>
+        <f t="shared" si="4"/>
         <v>10.4</v>
       </c>
       <c r="J68">
-        <f>F68-E68</f>
+        <f t="shared" si="5"/>
         <v>13.399999999999999</v>
       </c>
       <c r="L68" s="2">
@@ -13171,15 +13211,15 @@
         <v>62.9</v>
       </c>
       <c r="H69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.13</v>
       </c>
       <c r="I69">
-        <f>D69-C69</f>
+        <f t="shared" si="4"/>
         <v>14.600000000000001</v>
       </c>
       <c r="J69">
-        <f>F69-E69</f>
+        <f t="shared" si="5"/>
         <v>60.9</v>
       </c>
       <c r="L69" s="2">
@@ -13206,15 +13246,15 @@
         <v>0.1</v>
       </c>
       <c r="H70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.05</v>
       </c>
       <c r="I70">
-        <f>D70-C70</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J70">
-        <f>F70-E70</f>
+        <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
       <c r="L70" s="2">
@@ -13241,15 +13281,15 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="H71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.3</v>
       </c>
       <c r="I71">
-        <f>D71-C71</f>
+        <f t="shared" si="4"/>
         <v>15.1</v>
       </c>
       <c r="J71">
-        <f>F71-E71</f>
+        <f t="shared" si="5"/>
         <v>8.9</v>
       </c>
       <c r="L71" s="2">
@@ -13276,15 +13316,15 @@
         <v>1.2</v>
       </c>
       <c r="H72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="I72">
-        <f>D72-C72</f>
+        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
       <c r="J72">
-        <f>F72-E72</f>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="L72" s="2">
@@ -13311,15 +13351,15 @@
         <v>2.4</v>
       </c>
       <c r="H73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.12</v>
       </c>
       <c r="I73">
-        <f>D73-C73</f>
+        <f t="shared" si="4"/>
         <v>6.4</v>
       </c>
       <c r="J73">
-        <f>F73-E73</f>
+        <f t="shared" si="5"/>
         <v>2.4</v>
       </c>
       <c r="L73" s="2">
@@ -13346,15 +13386,15 @@
         <v>64.8</v>
       </c>
       <c r="H74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="I74">
-        <f>D74-C74</f>
+        <f t="shared" si="4"/>
         <v>17.799999999999997</v>
       </c>
       <c r="J74">
-        <f>F74-E74</f>
+        <f t="shared" si="5"/>
         <v>24.599999999999994</v>
       </c>
       <c r="L74" s="2">
@@ -13381,15 +13421,15 @@
         <v>1.7</v>
       </c>
       <c r="H75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="I75">
-        <f>D75-C75</f>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="J75">
-        <f>F75-E75</f>
+        <f t="shared" si="5"/>
         <v>1.7</v>
       </c>
       <c r="L75" s="2">
@@ -13416,15 +13456,15 @@
         <v>6</v>
       </c>
       <c r="H76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>8.9999999999999969E-2</v>
       </c>
       <c r="I76">
-        <f>D76-C76</f>
+        <f t="shared" si="4"/>
         <v>25.2</v>
       </c>
       <c r="J76">
-        <f>F76-E76</f>
+        <f t="shared" si="5"/>
         <v>5.6</v>
       </c>
       <c r="L76" s="2">
@@ -13451,15 +13491,15 @@
         <v>36.700000000000003</v>
       </c>
       <c r="H77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I77">
-        <f>D77-C77</f>
+        <f t="shared" si="4"/>
         <v>0.40000000000000568</v>
       </c>
       <c r="J77">
-        <f>F77-E77</f>
+        <f t="shared" si="5"/>
         <v>0.20000000000000284</v>
       </c>
       <c r="L77" s="2">
@@ -13486,15 +13526,15 @@
         <v>0.1</v>
       </c>
       <c r="H78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I78">
-        <f>D78-C78</f>
+        <f t="shared" si="4"/>
         <v>0.40000000000000013</v>
       </c>
       <c r="J78">
-        <f>F78-E78</f>
+        <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
       <c r="L78" s="2">
@@ -13521,15 +13561,15 @@
         <v>2.5</v>
       </c>
       <c r="H79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I79">
-        <f>D79-C79</f>
+        <f t="shared" si="4"/>
         <v>1.3000000000000007</v>
       </c>
       <c r="J79">
-        <f>F79-E79</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L79" s="2">
@@ -13556,15 +13596,15 @@
         <v>13</v>
       </c>
       <c r="H80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-5.0000000000000044E-2</v>
       </c>
       <c r="I80">
-        <f>D80-C80</f>
+        <f t="shared" si="4"/>
         <v>5.9000000000000021</v>
       </c>
       <c r="J80">
-        <f>F80-E80</f>
+        <f t="shared" si="5"/>
         <v>12.7</v>
       </c>
       <c r="L80" s="2">
@@ -13591,15 +13631,15 @@
         <v>4.2</v>
       </c>
       <c r="H81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="I81">
-        <f>D81-C81</f>
+        <f t="shared" si="4"/>
         <v>22.4</v>
       </c>
       <c r="J81">
-        <f>F81-E81</f>
+        <f t="shared" si="5"/>
         <v>4.2</v>
       </c>
       <c r="L81" s="2">
@@ -13626,15 +13666,15 @@
         <v>45.9</v>
       </c>
       <c r="H82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="I82">
-        <f>D82-C82</f>
+        <f t="shared" si="4"/>
         <v>8.0999999999999979</v>
       </c>
       <c r="J82">
-        <f>F82-E82</f>
+        <f t="shared" si="5"/>
         <v>43.199999999999996</v>
       </c>
       <c r="L82" s="2">
@@ -13661,15 +13701,15 @@
         <v>0.2</v>
       </c>
       <c r="H83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.02</v>
       </c>
       <c r="I83">
-        <f>D83-C83</f>
+        <f t="shared" si="4"/>
         <v>8.3999999999999986</v>
       </c>
       <c r="J83">
-        <f>F83-E83</f>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
       <c r="L83" s="2">
@@ -13696,15 +13736,15 @@
         <v>0</v>
       </c>
       <c r="H84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="I84">
-        <f>D84-C84</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J84">
-        <f>F84-E84</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L84" s="2">
@@ -13731,15 +13771,15 @@
         <v>3.3</v>
       </c>
       <c r="H85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.19999999999999973</v>
       </c>
       <c r="I85">
-        <f>D85-C85</f>
+        <f t="shared" si="4"/>
         <v>8.1000000000000014</v>
       </c>
       <c r="J85">
-        <f>F85-E85</f>
+        <f t="shared" si="5"/>
         <v>1.0999999999999996</v>
       </c>
       <c r="L85" s="2">
@@ -13766,15 +13806,15 @@
         <v>0</v>
       </c>
       <c r="H86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.12</v>
       </c>
       <c r="I86">
-        <f>D86-C86</f>
+        <f t="shared" si="4"/>
         <v>16.5</v>
       </c>
       <c r="J86">
-        <f>F86-E86</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L86" s="2">
@@ -13801,15 +13841,15 @@
         <v>3.9</v>
       </c>
       <c r="H87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.3600000000000003</v>
       </c>
       <c r="I87">
-        <f>D87-C87</f>
+        <f t="shared" si="4"/>
         <v>13.899999999999999</v>
       </c>
       <c r="J87">
-        <f>F87-E87</f>
+        <f t="shared" si="5"/>
         <v>3.9</v>
       </c>
       <c r="L87" s="2">
@@ -13836,15 +13876,15 @@
         <v>2.1</v>
       </c>
       <c r="H88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.30000000000000004</v>
       </c>
       <c r="I88">
-        <f>D88-C88</f>
+        <f t="shared" si="4"/>
         <v>0.70000000000000018</v>
       </c>
       <c r="J88">
-        <f>F88-E88</f>
+        <f t="shared" si="5"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="L88" s="2">
@@ -13871,15 +13911,15 @@
         <v>5.8</v>
       </c>
       <c r="H89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-1.1600000000000001</v>
       </c>
       <c r="I89">
-        <f>D89-C89</f>
+        <f t="shared" si="4"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="J89">
-        <f>F89-E89</f>
+        <f t="shared" si="5"/>
         <v>5.3999999999999995</v>
       </c>
       <c r="L89" s="2">
@@ -13906,15 +13946,15 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.65</v>
       </c>
       <c r="I90">
-        <f>D90-C90</f>
+        <f t="shared" si="4"/>
         <v>1.7000000000000002</v>
       </c>
       <c r="J90">
-        <f>F90-E90</f>
+        <f t="shared" si="5"/>
         <v>0.70000000000000018</v>
       </c>
       <c r="L90" s="2">
@@ -13941,15 +13981,15 @@
         <v>0</v>
       </c>
       <c r="H91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.11000000000000001</v>
       </c>
       <c r="I91">
-        <f>D91-C91</f>
+        <f t="shared" si="4"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="J91">
-        <f>F91-E91</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L91" s="2">
@@ -13976,15 +14016,15 @@
         <v>10.4</v>
       </c>
       <c r="H92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.0100000000000002</v>
       </c>
       <c r="I92">
-        <f>D92-C92</f>
+        <f t="shared" si="4"/>
         <v>14.200000000000001</v>
       </c>
       <c r="J92">
-        <f>F92-E92</f>
+        <f t="shared" si="5"/>
         <v>9.9</v>
       </c>
       <c r="L92" s="2">
@@ -14011,15 +14051,15 @@
         <v>0</v>
       </c>
       <c r="H93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I93">
-        <f>D93-C93</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J93">
-        <f>F93-E93</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L93" s="2">
@@ -14046,15 +14086,15 @@
         <v>0.3</v>
       </c>
       <c r="H94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99</v>
       </c>
       <c r="I94">
-        <f>D94-C94</f>
+        <f t="shared" si="4"/>
         <v>7.8999999999999986</v>
       </c>
       <c r="J94">
-        <f>F94-E94</f>
+        <f t="shared" si="5"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="L94" s="2">
@@ -14081,15 +14121,15 @@
         <v>20.100000000000001</v>
       </c>
       <c r="H95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="I95">
-        <f>D95-C95</f>
+        <f t="shared" si="4"/>
         <v>15.7</v>
       </c>
       <c r="J95">
-        <f>F95-E95</f>
+        <f t="shared" si="5"/>
         <v>19.5</v>
       </c>
       <c r="L95" s="2">
@@ -14116,15 +14156,15 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="H96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I96">
-        <f>D96-C96</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="J96">
-        <f>F96-E96</f>
+        <f t="shared" si="5"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="L96" s="2">
@@ -14151,15 +14191,15 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="H97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.05</v>
       </c>
       <c r="I97">
-        <f>D97-C97</f>
+        <f t="shared" si="4"/>
         <v>1.2999999999999972</v>
       </c>
       <c r="J97">
-        <f>F97-E97</f>
+        <f t="shared" si="5"/>
         <v>9.9999999999999645E-2</v>
       </c>
       <c r="L97" s="2">
@@ -14186,15 +14226,15 @@
         <v>30.1</v>
       </c>
       <c r="H98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I98">
-        <f>D98-C98</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J98">
-        <f>F98-E98</f>
+        <f t="shared" si="5"/>
         <v>30.1</v>
       </c>
       <c r="L98" s="2">
@@ -14221,15 +14261,15 @@
         <v>0</v>
       </c>
       <c r="H99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-6.0000000000000012E-2</v>
       </c>
       <c r="I99">
-        <f>D99-C99</f>
+        <f t="shared" si="4"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="J99">
-        <f>F99-E99</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L99" s="2">
@@ -14256,15 +14296,15 @@
         <v>10</v>
       </c>
       <c r="H100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-4.25</v>
       </c>
       <c r="I100">
-        <f>D100-C100</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J100">
-        <f>F100-E100</f>
+        <f t="shared" si="5"/>
         <v>6.3</v>
       </c>
       <c r="L100" s="2">
@@ -14291,15 +14331,15 @@
         <v>20.2</v>
       </c>
       <c r="H101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I101">
-        <f>D101-C101</f>
+        <f t="shared" si="4"/>
         <v>16.5</v>
       </c>
       <c r="J101">
-        <f>F101-E101</f>
+        <f t="shared" si="5"/>
         <v>19.899999999999999</v>
       </c>
       <c r="L101" s="2">
@@ -14326,15 +14366,15 @@
         <v>0.1</v>
       </c>
       <c r="H102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.45000000000000018</v>
       </c>
       <c r="I102">
-        <f>D102-C102</f>
+        <f t="shared" si="4"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="J102">
-        <f>F102-E102</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L102" s="2">
@@ -14361,15 +14401,15 @@
         <v>4.3</v>
       </c>
       <c r="H103">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-2.0000000000000004E-2</v>
       </c>
       <c r="I103">
-        <f>D103-C103</f>
+        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
       <c r="J103">
-        <f>F103-E103</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L103" s="2">
@@ -14396,15 +14436,15 @@
         <v>0.2</v>
       </c>
       <c r="H104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.75</v>
       </c>
       <c r="I104">
-        <f>D104-C104</f>
+        <f t="shared" si="4"/>
         <v>16.399999999999999</v>
       </c>
       <c r="J104">
-        <f>F104-E104</f>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
       <c r="L104" s="2">
@@ -14431,15 +14471,15 @@
         <v>0</v>
       </c>
       <c r="H105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.23</v>
       </c>
       <c r="I105">
-        <f>D105-C105</f>
+        <f t="shared" si="4"/>
         <v>0.60000000000000053</v>
       </c>
       <c r="J105">
-        <f>F105-E105</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L105" s="2">
@@ -14466,15 +14506,15 @@
         <v>0</v>
       </c>
       <c r="H106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-1.5</v>
       </c>
       <c r="I106">
-        <f>D106-C106</f>
+        <f t="shared" si="4"/>
         <v>15.2</v>
       </c>
       <c r="J106">
-        <f>F106-E106</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L106" s="2">
@@ -14501,15 +14541,15 @@
         <v>44.3</v>
       </c>
       <c r="H107">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-2.0000000000000018E-2</v>
       </c>
       <c r="I107">
-        <f>D107-C107</f>
+        <f t="shared" si="4"/>
         <v>11.6</v>
       </c>
       <c r="J107">
-        <f>F107-E107</f>
+        <f t="shared" si="5"/>
         <v>44.3</v>
       </c>
       <c r="L107" s="2">
@@ -14536,15 +14576,15 @@
         <v>0</v>
       </c>
       <c r="H108">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.31</v>
       </c>
       <c r="I108">
-        <f>D108-C108</f>
+        <f t="shared" si="4"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="J108">
-        <f>F108-E108</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L108" s="2">
@@ -14571,15 +14611,15 @@
         <v>0</v>
       </c>
       <c r="H109">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.54</v>
       </c>
       <c r="I109">
-        <f>D109-C109</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J109">
-        <f>F109-E109</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L109" s="2">
@@ -14606,15 +14646,15 @@
         <v>2</v>
       </c>
       <c r="H110">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="I110">
-        <f>D110-C110</f>
+        <f t="shared" si="4"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="J110">
-        <f>F110-E110</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L110" s="2">
@@ -14641,15 +14681,15 @@
         <v>4.3</v>
       </c>
       <c r="H111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I111">
-        <f>D111-C111</f>
+        <f t="shared" si="4"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="J111">
-        <f>F111-E111</f>
+        <f t="shared" si="5"/>
         <v>4.3</v>
       </c>
       <c r="L111" s="2">
@@ -14676,15 +14716,15 @@
         <v>0</v>
       </c>
       <c r="H112">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="I112">
-        <f>D112-C112</f>
+        <f t="shared" si="4"/>
         <v>4.0999999999999943</v>
       </c>
       <c r="J112">
-        <f>F112-E112</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L112" s="2">
@@ -14711,15 +14751,15 @@
         <v>30.6</v>
       </c>
       <c r="H113">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.13</v>
       </c>
       <c r="I113">
-        <f>D113-C113</f>
+        <f t="shared" si="4"/>
         <v>14.8</v>
       </c>
       <c r="J113">
-        <f>F113-E113</f>
+        <f t="shared" si="5"/>
         <v>30.400000000000002</v>
       </c>
       <c r="L113" s="2">
@@ -14746,15 +14786,15 @@
         <v>0</v>
       </c>
       <c r="H114">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.03</v>
       </c>
       <c r="I114">
-        <f>D114-C114</f>
+        <f t="shared" si="4"/>
         <v>22.5</v>
       </c>
       <c r="J114">
-        <f>F114-E114</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L114" s="2">
@@ -14781,15 +14821,15 @@
         <v>0</v>
       </c>
       <c r="H115">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.21999999999999997</v>
       </c>
       <c r="I115">
-        <f>D115-C115</f>
+        <f t="shared" si="4"/>
         <v>1.5</v>
       </c>
       <c r="J115">
-        <f>F115-E115</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L115" s="2">
@@ -14816,15 +14856,15 @@
         <v>3.4</v>
       </c>
       <c r="H116">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.21000000000000002</v>
       </c>
       <c r="I116">
-        <f>D116-C116</f>
+        <f t="shared" si="4"/>
         <v>2.6</v>
       </c>
       <c r="J116">
-        <f>F116-E116</f>
+        <f t="shared" si="5"/>
         <v>3.4</v>
       </c>
       <c r="L116" s="2">
@@ -14851,15 +14891,15 @@
         <v>0</v>
       </c>
       <c r="H117">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-5.0000000000000044E-2</v>
       </c>
       <c r="I117">
-        <f>D117-C117</f>
+        <f t="shared" si="4"/>
         <v>1.8000000000000007</v>
       </c>
       <c r="J117">
-        <f>F117-E117</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L117" s="2">
@@ -14886,15 +14926,15 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="H118">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.54</v>
       </c>
       <c r="I118">
-        <f>D118-C118</f>
+        <f t="shared" si="4"/>
         <v>1.1999999999999993</v>
       </c>
       <c r="J118">
-        <f>F118-E118</f>
+        <f t="shared" si="5"/>
         <v>0.79999999999999982</v>
       </c>
       <c r="L118" s="2">
@@ -14921,15 +14961,15 @@
         <v>0.4</v>
       </c>
       <c r="H119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I119">
-        <f>D119-C119</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="J119">
-        <f>F119-E119</f>
+        <f t="shared" si="5"/>
         <v>0.4</v>
       </c>
       <c r="L119" s="2">
@@ -14956,15 +14996,15 @@
         <v>0</v>
       </c>
       <c r="H120">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.22999999999999998</v>
       </c>
       <c r="I120">
-        <f>D120-C120</f>
+        <f t="shared" si="4"/>
         <v>4.6000000000000005</v>
       </c>
       <c r="J120">
-        <f>F120-E120</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L120" s="2">
@@ -14991,15 +15031,15 @@
         <v>4.7</v>
       </c>
       <c r="H121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I121">
-        <f>D121-C121</f>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="J121">
-        <f>F121-E121</f>
+        <f t="shared" si="5"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="L121" s="2">
@@ -15026,15 +15066,15 @@
         <v>3.4</v>
       </c>
       <c r="H122">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.28000000000000003</v>
       </c>
       <c r="I122">
-        <f>D122-C122</f>
+        <f t="shared" si="4"/>
         <v>7.7</v>
       </c>
       <c r="J122">
-        <f>F122-E122</f>
+        <f t="shared" si="5"/>
         <v>3.4</v>
       </c>
       <c r="L122" s="2">
@@ -15061,15 +15101,15 @@
         <v>32.299999999999997</v>
       </c>
       <c r="H123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.39000000000000012</v>
       </c>
       <c r="I123">
-        <f>D123-C123</f>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="J123">
-        <f>F123-E123</f>
+        <f t="shared" si="5"/>
         <v>9.9999999999994316E-2</v>
       </c>
       <c r="L123" s="2">
@@ -15096,15 +15136,15 @@
         <v>0.3</v>
       </c>
       <c r="H124">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.74</v>
       </c>
       <c r="I124">
-        <f>D124-C124</f>
+        <f t="shared" si="4"/>
         <v>4.0999999999999996</v>
       </c>
       <c r="J124">
-        <f>F124-E124</f>
+        <f t="shared" si="5"/>
         <v>0.3</v>
       </c>
       <c r="L124" s="2">
@@ -15131,15 +15171,15 @@
         <v>19</v>
       </c>
       <c r="H125">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.10000000000000003</v>
       </c>
       <c r="I125">
-        <f>D125-C125</f>
+        <f t="shared" si="4"/>
         <v>10.5</v>
       </c>
       <c r="J125">
-        <f>F125-E125</f>
+        <f t="shared" si="5"/>
         <v>17.399999999999999</v>
       </c>
       <c r="L125" s="2">
@@ -15166,15 +15206,15 @@
         <v>0.1</v>
       </c>
       <c r="H126">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-0.06</v>
       </c>
       <c r="I126">
-        <f>D126-C126</f>
+        <f t="shared" si="4"/>
         <v>1.2999999999999998</v>
       </c>
       <c r="J126">
-        <f>F126-E126</f>
+        <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
       <c r="L126" s="2">
@@ -15201,15 +15241,15 @@
         <v>0</v>
       </c>
       <c r="H127">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-1.4100000000000001</v>
       </c>
       <c r="I127">
-        <f>D127-C127</f>
+        <f t="shared" si="4"/>
         <v>2.8</v>
       </c>
       <c r="J127">
-        <f>F127-E127</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L127" s="2">
@@ -15236,15 +15276,15 @@
         <v>100.3</v>
       </c>
       <c r="H128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I128">
-        <f>D128-C128</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="J128">
-        <f>F128-E128</f>
+        <f t="shared" si="5"/>
         <v>100.2</v>
       </c>
       <c r="L128" s="2">
@@ -15271,15 +15311,15 @@
         <v>0</v>
       </c>
       <c r="H129">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-1.1300000000000001</v>
       </c>
       <c r="I129">
-        <f>D129-C129</f>
+        <f t="shared" si="4"/>
         <v>13.1</v>
       </c>
       <c r="J129">
-        <f>F129-E129</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L129" s="2">
@@ -15306,15 +15346,15 @@
         <v>0</v>
       </c>
       <c r="H130">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-1.87</v>
       </c>
       <c r="I130">
-        <f>D130-C130</f>
+        <f t="shared" ref="I130:I193" si="7">D130-C130</f>
         <v>1.4999999999999996</v>
       </c>
       <c r="J130">
-        <f>F130-E130</f>
+        <f t="shared" ref="J130:J193" si="8">F130-E130</f>
         <v>0</v>
       </c>
       <c r="L130" s="2">
@@ -15341,15 +15381,15 @@
         <v>1.3</v>
       </c>
       <c r="H131">
-        <f t="shared" ref="H131:H194" si="3">B131-A131</f>
+        <f t="shared" ref="H131:H194" si="9">B131-A131</f>
         <v>-0.73000000000000009</v>
       </c>
       <c r="I131">
-        <f>D131-C131</f>
+        <f t="shared" si="7"/>
         <v>33.4</v>
       </c>
       <c r="J131">
-        <f>F131-E131</f>
+        <f t="shared" si="8"/>
         <v>1.3</v>
       </c>
       <c r="L131" s="2">
@@ -15376,15 +15416,15 @@
         <v>18</v>
       </c>
       <c r="H132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="I132">
-        <f>D132-C132</f>
+        <f t="shared" si="7"/>
         <v>3.6999999999999993</v>
       </c>
       <c r="J132">
-        <f>F132-E132</f>
+        <f t="shared" si="8"/>
         <v>16.2</v>
       </c>
       <c r="L132" s="2">
@@ -15411,15 +15451,15 @@
         <v>0.2</v>
       </c>
       <c r="H133">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="I133">
-        <f>D133-C133</f>
+        <f t="shared" si="7"/>
         <v>4.2</v>
       </c>
       <c r="J133">
-        <f>F133-E133</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L133" s="2">
@@ -15446,15 +15486,15 @@
         <v>28.1</v>
       </c>
       <c r="H134">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.12</v>
       </c>
       <c r="I134">
-        <f>D134-C134</f>
+        <f t="shared" si="7"/>
         <v>26.299999999999997</v>
       </c>
       <c r="J134">
-        <f>F134-E134</f>
+        <f t="shared" si="8"/>
         <v>27.6</v>
       </c>
       <c r="L134" s="2">
@@ -15481,15 +15521,15 @@
         <v>0</v>
       </c>
       <c r="H135">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-1.6199999999999999</v>
       </c>
       <c r="I135">
-        <f>D135-C135</f>
+        <f t="shared" si="7"/>
         <v>15.2</v>
       </c>
       <c r="J135">
-        <f>F135-E135</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L135" s="2">
@@ -15516,15 +15556,15 @@
         <v>57.7</v>
       </c>
       <c r="H136">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="I136">
-        <f>D136-C136</f>
+        <f t="shared" si="7"/>
         <v>7.1999999999999993</v>
       </c>
       <c r="J136">
-        <f>F136-E136</f>
+        <f t="shared" si="8"/>
         <v>36.5</v>
       </c>
       <c r="L136" s="2">
@@ -15551,15 +15591,15 @@
         <v>56.6</v>
       </c>
       <c r="H137">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I137">
-        <f>D137-C137</f>
+        <f t="shared" si="7"/>
         <v>48.199999999999996</v>
       </c>
       <c r="J137">
-        <f>F137-E137</f>
+        <f t="shared" si="8"/>
         <v>56</v>
       </c>
       <c r="L137" s="2">
@@ -15586,15 +15626,15 @@
         <v>12.5</v>
       </c>
       <c r="H138">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.48</v>
       </c>
       <c r="I138">
-        <f>D138-C138</f>
+        <f t="shared" si="7"/>
         <v>7.8000000000000007</v>
       </c>
       <c r="J138">
-        <f>F138-E138</f>
+        <f t="shared" si="8"/>
         <v>7.8</v>
       </c>
       <c r="L138" s="2">
@@ -15621,15 +15661,15 @@
         <v>37.700000000000003</v>
       </c>
       <c r="H139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-0.32999999999999985</v>
       </c>
       <c r="I139">
-        <f>D139-C139</f>
+        <f t="shared" si="7"/>
         <v>21.700000000000003</v>
       </c>
       <c r="J139">
-        <f>F139-E139</f>
+        <f t="shared" si="8"/>
         <v>37.1</v>
       </c>
       <c r="L139" s="2">
@@ -15656,15 +15696,15 @@
         <v>0</v>
       </c>
       <c r="H140">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-2.74</v>
       </c>
       <c r="I140">
-        <f>D140-C140</f>
+        <f t="shared" si="7"/>
         <v>9.9000000000000021</v>
       </c>
       <c r="J140">
-        <f>F140-E140</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L140" s="2">
@@ -15691,15 +15731,15 @@
         <v>0.2</v>
       </c>
       <c r="H141">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.44</v>
       </c>
       <c r="I141">
-        <f>D141-C141</f>
+        <f t="shared" si="7"/>
         <v>2.5999999999999996</v>
       </c>
       <c r="J141">
-        <f>F141-E141</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L141" s="2">
@@ -15726,15 +15766,15 @@
         <v>20.399999999999999</v>
       </c>
       <c r="H142">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-8.9999999999999969E-2</v>
       </c>
       <c r="I142">
-        <f>D142-C142</f>
+        <f t="shared" si="7"/>
         <v>2.0999999999999996</v>
       </c>
       <c r="J142">
-        <f>F142-E142</f>
+        <f t="shared" si="8"/>
         <v>20.299999999999997</v>
       </c>
       <c r="L142" s="2">
@@ -15761,15 +15801,15 @@
         <v>60.7</v>
       </c>
       <c r="H143">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-0.02</v>
       </c>
       <c r="I143">
-        <f>D143-C143</f>
+        <f t="shared" si="7"/>
         <v>11.399999999999999</v>
       </c>
       <c r="J143">
-        <f>F143-E143</f>
+        <f t="shared" si="8"/>
         <v>10.100000000000001</v>
       </c>
       <c r="L143" s="2">
@@ -15796,15 +15836,15 @@
         <v>1.3</v>
       </c>
       <c r="H144">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I144">
-        <f>D144-C144</f>
+        <f t="shared" si="7"/>
         <v>10.7</v>
       </c>
       <c r="J144">
-        <f>F144-E144</f>
+        <f t="shared" si="8"/>
         <v>1.3</v>
       </c>
       <c r="L144" s="2">
@@ -15831,15 +15871,15 @@
         <v>5.6</v>
       </c>
       <c r="H145">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.63000000000000012</v>
       </c>
       <c r="I145">
-        <f>D145-C145</f>
+        <f t="shared" si="7"/>
         <v>0.70000000000000107</v>
       </c>
       <c r="J145">
-        <f>F145-E145</f>
+        <f t="shared" si="8"/>
         <v>3.8</v>
       </c>
       <c r="L145" s="2">
@@ -15866,15 +15906,15 @@
         <v>31.4</v>
       </c>
       <c r="H146">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="I146">
-        <f>D146-C146</f>
+        <f t="shared" si="7"/>
         <v>15.7</v>
       </c>
       <c r="J146">
-        <f>F146-E146</f>
+        <f t="shared" si="8"/>
         <v>30.9</v>
       </c>
       <c r="L146" s="2">
@@ -15901,15 +15941,15 @@
         <v>7.4</v>
       </c>
       <c r="H147">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I147">
-        <f>D147-C147</f>
+        <f t="shared" si="7"/>
         <v>2.4000000000000021</v>
       </c>
       <c r="J147">
-        <f>F147-E147</f>
+        <f t="shared" si="8"/>
         <v>3.6000000000000005</v>
       </c>
       <c r="L147" s="2">
@@ -15936,15 +15976,15 @@
         <v>0.4</v>
       </c>
       <c r="H148">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I148">
-        <f>D148-C148</f>
+        <f t="shared" si="7"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="J148">
-        <f>F148-E148</f>
+        <f t="shared" si="8"/>
         <v>0.10000000000000003</v>
       </c>
       <c r="L148" s="2">
@@ -15971,15 +16011,15 @@
         <v>0</v>
       </c>
       <c r="H149">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.67</v>
       </c>
       <c r="I149">
-        <f>D149-C149</f>
+        <f t="shared" si="7"/>
         <v>3.6</v>
       </c>
       <c r="J149">
-        <f>F149-E149</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L149" s="2">
@@ -16006,15 +16046,15 @@
         <v>6.8</v>
       </c>
       <c r="H150">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-4.0000000000000008E-2</v>
       </c>
       <c r="I150">
-        <f>D150-C150</f>
+        <f t="shared" si="7"/>
         <v>26.599999999999998</v>
       </c>
       <c r="J150">
-        <f>F150-E150</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="L150" s="2">
@@ -16041,15 +16081,15 @@
         <v>2.5</v>
       </c>
       <c r="H151">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-0.20000000000000007</v>
       </c>
       <c r="I151">
-        <f>D151-C151</f>
+        <f t="shared" si="7"/>
         <v>2.3000000000000007</v>
       </c>
       <c r="J151">
-        <f>F151-E151</f>
+        <f t="shared" si="8"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="L151" s="2">
@@ -16076,15 +16116,15 @@
         <v>52.7</v>
       </c>
       <c r="H152">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="I152">
-        <f>D152-C152</f>
+        <f t="shared" si="7"/>
         <v>18.899999999999999</v>
       </c>
       <c r="J152">
-        <f>F152-E152</f>
+        <f t="shared" si="8"/>
         <v>51.300000000000004</v>
       </c>
       <c r="L152" s="2">
@@ -16111,15 +16151,15 @@
         <v>5.5</v>
       </c>
       <c r="H153">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.06</v>
       </c>
       <c r="I153">
-        <f>D153-C153</f>
+        <f t="shared" si="7"/>
         <v>13.700000000000001</v>
       </c>
       <c r="J153">
-        <f>F153-E153</f>
+        <f t="shared" si="8"/>
         <v>1.4000000000000004</v>
       </c>
       <c r="L153" s="2">
@@ -16146,15 +16186,15 @@
         <v>1.8</v>
       </c>
       <c r="H154">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.9499999999999997</v>
       </c>
       <c r="I154">
-        <f>D154-C154</f>
+        <f t="shared" si="7"/>
         <v>0.30000000000000071</v>
       </c>
       <c r="J154">
-        <f>F154-E154</f>
+        <f t="shared" si="8"/>
         <v>0.10000000000000009</v>
       </c>
       <c r="L154" s="2">
@@ -16181,15 +16221,15 @@
         <v>1.6</v>
       </c>
       <c r="H155">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I155">
-        <f>D155-C155</f>
+        <f t="shared" si="7"/>
         <v>1.4000000000000001</v>
       </c>
       <c r="J155">
-        <f>F155-E155</f>
+        <f t="shared" si="8"/>
         <v>1.6</v>
       </c>
       <c r="L155" s="2">
@@ -16216,15 +16256,15 @@
         <v>42.8</v>
       </c>
       <c r="H156">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-0.51</v>
       </c>
       <c r="I156">
-        <f>D156-C156</f>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
       <c r="J156">
-        <f>F156-E156</f>
+        <f t="shared" si="8"/>
         <v>41.3</v>
       </c>
       <c r="L156" s="2">
@@ -16251,15 +16291,15 @@
         <v>11.5</v>
       </c>
       <c r="H157">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-0.05</v>
       </c>
       <c r="I157">
-        <f>D157-C157</f>
+        <f t="shared" si="7"/>
         <v>6.4</v>
       </c>
       <c r="J157">
-        <f>F157-E157</f>
+        <f t="shared" si="8"/>
         <v>9.1999999999999993</v>
       </c>
       <c r="L157" s="2">
@@ -16286,15 +16326,15 @@
         <v>0</v>
       </c>
       <c r="H158">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-1.46</v>
       </c>
       <c r="I158">
-        <f>D158-C158</f>
+        <f t="shared" si="7"/>
         <v>0.59999999999999964</v>
       </c>
       <c r="J158">
-        <f>F158-E158</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L158" s="2">
@@ -16321,15 +16361,15 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="H159">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.78</v>
       </c>
       <c r="I159">
-        <f>D159-C159</f>
+        <f t="shared" si="7"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="J159">
-        <f>F159-E159</f>
+        <f t="shared" si="8"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="L159" s="2">
@@ -16356,15 +16396,15 @@
         <v>0</v>
       </c>
       <c r="H160">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I160">
-        <f>D160-C160</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J160">
-        <f>F160-E160</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L160" s="2">
@@ -16391,15 +16431,15 @@
         <v>0</v>
       </c>
       <c r="H161">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="I161">
-        <f>D161-C161</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J161">
-        <f>F161-E161</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L161" s="2">
@@ -16426,15 +16466,15 @@
         <v>3.4</v>
       </c>
       <c r="H162">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I162">
-        <f>D162-C162</f>
+        <f t="shared" si="7"/>
         <v>23.700000000000003</v>
       </c>
       <c r="J162">
-        <f>F162-E162</f>
+        <f t="shared" si="8"/>
         <v>2.8</v>
       </c>
       <c r="L162" s="2">
@@ -16461,15 +16501,15 @@
         <v>14.4</v>
       </c>
       <c r="H163">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-1.0000000000000009E-2</v>
       </c>
       <c r="I163">
-        <f>D163-C163</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J163">
-        <f>F163-E163</f>
+        <f t="shared" si="8"/>
         <v>6.3000000000000007</v>
       </c>
       <c r="L163" s="2">
@@ -16496,15 +16536,15 @@
         <v>0</v>
       </c>
       <c r="H164">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-0.63</v>
       </c>
       <c r="I164">
-        <f>D164-C164</f>
+        <f t="shared" si="7"/>
         <v>3.0999999999999996</v>
       </c>
       <c r="J164">
-        <f>F164-E164</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L164" s="2">
@@ -16531,15 +16571,15 @@
         <v>1</v>
       </c>
       <c r="H165">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I165">
-        <f>D165-C165</f>
+        <f t="shared" si="7"/>
         <v>0.10000000000000142</v>
       </c>
       <c r="J165">
-        <f>F165-E165</f>
+        <f t="shared" si="8"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="L165" s="2">
@@ -16566,15 +16606,15 @@
         <v>7.8</v>
       </c>
       <c r="H166">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-0.92</v>
       </c>
       <c r="I166">
-        <f>D166-C166</f>
+        <f t="shared" si="7"/>
         <v>8.1000000000000014</v>
       </c>
       <c r="J166">
-        <f>F166-E166</f>
+        <f t="shared" si="8"/>
         <v>7.8</v>
       </c>
       <c r="L166" s="2">
@@ -16601,15 +16641,15 @@
         <v>1.5</v>
       </c>
       <c r="H167">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I167">
-        <f>D167-C167</f>
+        <f t="shared" si="7"/>
         <v>0.39999999999999947</v>
       </c>
       <c r="J167">
-        <f>F167-E167</f>
+        <f t="shared" si="8"/>
         <v>1.5</v>
       </c>
       <c r="L167" s="2">
@@ -16636,15 +16676,15 @@
         <v>0</v>
       </c>
       <c r="H168">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-0.08</v>
       </c>
       <c r="I168">
-        <f>D168-C168</f>
+        <f t="shared" si="7"/>
         <v>21.8</v>
       </c>
       <c r="J168">
-        <f>F168-E168</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L168" s="2">
@@ -16671,15 +16711,15 @@
         <v>98.5</v>
       </c>
       <c r="H169">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="I169">
-        <f>D169-C169</f>
+        <f t="shared" si="7"/>
         <v>46.300000000000004</v>
       </c>
       <c r="J169">
-        <f>F169-E169</f>
+        <f t="shared" si="8"/>
         <v>98.5</v>
       </c>
       <c r="L169" s="2">
@@ -16706,15 +16746,15 @@
         <v>0.9</v>
       </c>
       <c r="H170">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="I170">
-        <f>D170-C170</f>
+        <f t="shared" si="7"/>
         <v>2.1</v>
       </c>
       <c r="J170">
-        <f>F170-E170</f>
+        <f t="shared" si="8"/>
         <v>0.9</v>
       </c>
       <c r="L170" s="2">
@@ -16741,15 +16781,15 @@
         <v>0</v>
       </c>
       <c r="H171">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.13000000000000012</v>
       </c>
       <c r="I171">
-        <f>D171-C171</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J171">
-        <f>F171-E171</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L171" s="2">
@@ -16776,15 +16816,15 @@
         <v>13.4</v>
       </c>
       <c r="H172">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I172">
-        <f>D172-C172</f>
+        <f t="shared" si="7"/>
         <v>3.2</v>
       </c>
       <c r="J172">
-        <f>F172-E172</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="L172" s="2">
@@ -16811,15 +16851,15 @@
         <v>0</v>
       </c>
       <c r="H173">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I173">
-        <f>D173-C173</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="J173">
-        <f>F173-E173</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L173" s="2">
@@ -16846,15 +16886,15 @@
         <v>7.5</v>
       </c>
       <c r="H174">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.5499999999999998</v>
       </c>
       <c r="I174">
-        <f>D174-C174</f>
+        <f t="shared" si="7"/>
         <v>19.899999999999999</v>
       </c>
       <c r="J174">
-        <f>F174-E174</f>
+        <f t="shared" si="8"/>
         <v>6.7</v>
       </c>
       <c r="L174" s="2">
@@ -16881,15 +16921,15 @@
         <v>1.3</v>
       </c>
       <c r="H175">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-2.9999999999999971E-2</v>
       </c>
       <c r="I175">
-        <f>D175-C175</f>
+        <f t="shared" si="7"/>
         <v>2.8999999999999986</v>
       </c>
       <c r="J175">
-        <f>F175-E175</f>
+        <f t="shared" si="8"/>
         <v>1.2</v>
       </c>
       <c r="L175" s="2">
@@ -16916,15 +16956,15 @@
         <v>0.5</v>
       </c>
       <c r="H176">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I176">
-        <f>D176-C176</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J176">
-        <f>F176-E176</f>
+        <f t="shared" si="8"/>
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="L176" s="2">
@@ -16951,15 +16991,15 @@
         <v>0.2</v>
       </c>
       <c r="H177">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>9.9999999999999534E-3</v>
       </c>
       <c r="I177">
-        <f>D177-C177</f>
+        <f t="shared" si="7"/>
         <v>2.5999999999999979</v>
       </c>
       <c r="J177">
-        <f>F177-E177</f>
+        <f t="shared" si="8"/>
         <v>0.1</v>
       </c>
       <c r="L177" s="2">
@@ -16986,15 +17026,15 @@
         <v>0</v>
       </c>
       <c r="H178">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I178">
-        <f>D178-C178</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J178">
-        <f>F178-E178</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L178" s="2">
@@ -17021,15 +17061,15 @@
         <v>1.2</v>
       </c>
       <c r="H179">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="I179">
-        <f>D179-C179</f>
+        <f t="shared" si="7"/>
         <v>2.6000000000000014</v>
       </c>
       <c r="J179">
-        <f>F179-E179</f>
+        <f t="shared" si="8"/>
         <v>-0.10000000000000009</v>
       </c>
       <c r="L179" s="2">
@@ -17056,15 +17096,15 @@
         <v>0</v>
       </c>
       <c r="H180">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.12</v>
       </c>
       <c r="I180">
-        <f>D180-C180</f>
+        <f t="shared" si="7"/>
         <v>0.39999999999999991</v>
       </c>
       <c r="J180">
-        <f>F180-E180</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L180" s="2">
@@ -17091,15 +17131,15 @@
         <v>22.9</v>
       </c>
       <c r="H181">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I181">
-        <f>D181-C181</f>
+        <f t="shared" si="7"/>
         <v>11.2</v>
       </c>
       <c r="J181">
-        <f>F181-E181</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L181" s="2">
@@ -17126,15 +17166,15 @@
         <v>0</v>
       </c>
       <c r="H182">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.10000000000000009</v>
       </c>
       <c r="I182">
-        <f>D182-C182</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J182">
-        <f>F182-E182</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L182" s="2">
@@ -17161,15 +17201,15 @@
         <v>10.5</v>
       </c>
       <c r="H183">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.06</v>
       </c>
       <c r="I183">
-        <f>D183-C183</f>
+        <f t="shared" si="7"/>
         <v>8.5</v>
       </c>
       <c r="J183">
-        <f>F183-E183</f>
+        <f t="shared" si="8"/>
         <v>6.4</v>
       </c>
       <c r="L183" s="2">
@@ -17196,15 +17236,15 @@
         <v>0</v>
       </c>
       <c r="H184">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.999999999999998E-2</v>
       </c>
       <c r="I184">
-        <f>D184-C184</f>
+        <f t="shared" si="7"/>
         <v>9.2000000000000011</v>
       </c>
       <c r="J184">
-        <f>F184-E184</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L184" s="2">
@@ -17231,15 +17271,15 @@
         <v>0.6</v>
       </c>
       <c r="H185">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.65</v>
       </c>
       <c r="I185">
-        <f>D185-C185</f>
+        <f t="shared" si="7"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="J185">
-        <f>F185-E185</f>
+        <f t="shared" si="8"/>
         <v>0.6</v>
       </c>
       <c r="L185" s="2">
@@ -17266,15 +17306,15 @@
         <v>0</v>
       </c>
       <c r="H186">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.0000000000000004E-2</v>
       </c>
       <c r="I186">
-        <f>D186-C186</f>
+        <f t="shared" si="7"/>
         <v>19.299999999999997</v>
       </c>
       <c r="J186">
-        <f>F186-E186</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L186" s="2">
@@ -17301,15 +17341,15 @@
         <v>18.2</v>
       </c>
       <c r="H187">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6.0000000000000053E-2</v>
       </c>
       <c r="I187">
-        <f>D187-C187</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="J187">
-        <f>F187-E187</f>
+        <f t="shared" si="8"/>
         <v>14.5</v>
       </c>
       <c r="L187" s="2">
@@ -17336,15 +17376,15 @@
         <v>5.2</v>
       </c>
       <c r="H188">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="I188">
-        <f>D188-C188</f>
+        <f t="shared" si="7"/>
         <v>6.9</v>
       </c>
       <c r="J188">
-        <f>F188-E188</f>
+        <f t="shared" si="8"/>
         <v>1.3000000000000003</v>
       </c>
       <c r="L188" s="2">
@@ -17371,15 +17411,15 @@
         <v>3.8</v>
       </c>
       <c r="H189">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.22999999999999998</v>
       </c>
       <c r="I189">
-        <f>D189-C189</f>
+        <f t="shared" si="7"/>
         <v>8.6999999999999993</v>
       </c>
       <c r="J189">
-        <f>F189-E189</f>
+        <f t="shared" si="8"/>
         <v>3.8</v>
       </c>
       <c r="L189" s="2">
@@ -17406,15 +17446,15 @@
         <v>2.8</v>
       </c>
       <c r="H190">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.7699999999999996</v>
       </c>
       <c r="I190">
-        <f>D190-C190</f>
+        <f t="shared" si="7"/>
         <v>13.9</v>
       </c>
       <c r="J190">
-        <f>F190-E190</f>
+        <f t="shared" si="8"/>
         <v>2.8</v>
       </c>
       <c r="L190" s="2">
@@ -17441,15 +17481,15 @@
         <v>9.6</v>
       </c>
       <c r="H191">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I191">
-        <f>D191-C191</f>
+        <f t="shared" si="7"/>
         <v>14.4</v>
       </c>
       <c r="J191">
-        <f>F191-E191</f>
+        <f t="shared" si="8"/>
         <v>9.6</v>
       </c>
       <c r="L191" s="2">
@@ -17476,15 +17516,15 @@
         <v>3</v>
       </c>
       <c r="H192">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-0.32999999999999996</v>
       </c>
       <c r="I192">
-        <f>D192-C192</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J192">
-        <f>F192-E192</f>
+        <f t="shared" si="8"/>
         <v>2.8</v>
       </c>
       <c r="L192" s="2">
@@ -17511,15 +17551,15 @@
         <v>2.7</v>
       </c>
       <c r="H193">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.21</v>
       </c>
       <c r="I193">
-        <f>D193-C193</f>
+        <f t="shared" si="7"/>
         <v>4.1000000000000005</v>
       </c>
       <c r="J193">
-        <f>F193-E193</f>
+        <f t="shared" si="8"/>
         <v>1.6</v>
       </c>
       <c r="L193" s="2">
@@ -17546,15 +17586,15 @@
         <v>0.4</v>
       </c>
       <c r="H194">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>-0.37</v>
       </c>
       <c r="I194">
-        <f>D194-C194</f>
+        <f t="shared" ref="I194:I212" si="10">D194-C194</f>
         <v>0.2</v>
       </c>
       <c r="J194">
-        <f>F194-E194</f>
+        <f t="shared" ref="J194:J212" si="11">F194-E194</f>
         <v>0.4</v>
       </c>
       <c r="L194" s="2">
@@ -17581,15 +17621,15 @@
         <v>0</v>
       </c>
       <c r="H195">
-        <f t="shared" ref="H195:H212" si="4">B195-A195</f>
+        <f t="shared" ref="H195:H212" si="12">B195-A195</f>
         <v>0</v>
       </c>
       <c r="I195">
-        <f>D195-C195</f>
+        <f t="shared" si="10"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="J195">
-        <f>F195-E195</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L195" s="2">
@@ -17616,15 +17656,15 @@
         <v>1</v>
       </c>
       <c r="H196">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I196">
-        <f>D196-C196</f>
+        <f t="shared" si="10"/>
         <v>7.8999999999999986</v>
       </c>
       <c r="J196">
-        <f>F196-E196</f>
+        <f t="shared" si="11"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="L196" s="2">
@@ -17651,15 +17691,15 @@
         <v>0.3</v>
       </c>
       <c r="H197">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I197">
-        <f>D197-C197</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J197">
-        <f>F197-E197</f>
+        <f t="shared" si="11"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="L197" s="2">
@@ -17686,15 +17726,15 @@
         <v>0</v>
       </c>
       <c r="H198">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2.0299999999999998</v>
       </c>
       <c r="I198">
-        <f>D198-C198</f>
+        <f t="shared" si="10"/>
         <v>3.6999999999999993</v>
       </c>
       <c r="J198">
-        <f>F198-E198</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L198" s="2">
@@ -17721,15 +17761,15 @@
         <v>10.7</v>
       </c>
       <c r="H199">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0.15</v>
       </c>
       <c r="I199">
-        <f>D199-C199</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J199">
-        <f>F199-E199</f>
+        <f t="shared" si="11"/>
         <v>4.7999999999999989</v>
       </c>
       <c r="L199" s="2">
@@ -17756,15 +17796,15 @@
         <v>21</v>
       </c>
       <c r="H200">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2.11</v>
       </c>
       <c r="I200">
-        <f>D200-C200</f>
+        <f t="shared" si="10"/>
         <v>6.0000000000000018</v>
       </c>
       <c r="J200">
-        <f>F200-E200</f>
+        <f t="shared" si="11"/>
         <v>20.7</v>
       </c>
       <c r="L200" s="2">
@@ -17791,15 +17831,15 @@
         <v>17.2</v>
       </c>
       <c r="H201">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="I201">
-        <f>D201-C201</f>
+        <f t="shared" si="10"/>
         <v>6.5999999999999979</v>
       </c>
       <c r="J201">
-        <f>F201-E201</f>
+        <f t="shared" si="11"/>
         <v>12.2</v>
       </c>
       <c r="L201" s="2">
@@ -17826,15 +17866,15 @@
         <v>31.7</v>
       </c>
       <c r="H202">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>-0.1</v>
       </c>
       <c r="I202">
-        <f>D202-C202</f>
+        <f t="shared" si="10"/>
         <v>0.20000000000000107</v>
       </c>
       <c r="J202">
-        <f>F202-E202</f>
+        <f t="shared" si="11"/>
         <v>9.0999999999999979</v>
       </c>
       <c r="L202" s="2">
@@ -17861,15 +17901,15 @@
         <v>1.8</v>
       </c>
       <c r="H203">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>3.54</v>
       </c>
       <c r="I203">
-        <f>D203-C203</f>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="J203">
-        <f>F203-E203</f>
+        <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
       <c r="L203" s="2">
@@ -17896,15 +17936,15 @@
         <v>0</v>
       </c>
       <c r="H204">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0.52</v>
       </c>
       <c r="I204">
-        <f>D204-C204</f>
+        <f t="shared" si="10"/>
         <v>1.2999999999999998</v>
       </c>
       <c r="J204">
-        <f>F204-E204</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L204" s="2">
@@ -17931,15 +17971,15 @@
         <v>0</v>
       </c>
       <c r="H205">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I205">
-        <f>D205-C205</f>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="J205">
-        <f>F205-E205</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L205" s="2">
@@ -17966,15 +18006,15 @@
         <v>16.8</v>
       </c>
       <c r="H206">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>-0.22999999999999993</v>
       </c>
       <c r="I206">
-        <f>D206-C206</f>
+        <f t="shared" si="10"/>
         <v>13.899999999999999</v>
       </c>
       <c r="J206">
-        <f>F206-E206</f>
+        <f t="shared" si="11"/>
         <v>9.1000000000000014</v>
       </c>
       <c r="L206" s="2">
@@ -18001,15 +18041,15 @@
         <v>1.8</v>
       </c>
       <c r="H207">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0.72999999999999976</v>
       </c>
       <c r="I207">
-        <f>D207-C207</f>
+        <f t="shared" si="10"/>
         <v>1.9000000000000004</v>
       </c>
       <c r="J207">
-        <f>F207-E207</f>
+        <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
       <c r="L207" s="2">
@@ -18036,15 +18076,15 @@
         <v>2</v>
       </c>
       <c r="H208">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>-0.39999999999999991</v>
       </c>
       <c r="I208">
-        <f>D208-C208</f>
+        <f t="shared" si="10"/>
         <v>0.40000000000000036</v>
       </c>
       <c r="J208">
-        <f>F208-E208</f>
+        <f t="shared" si="11"/>
         <v>0.39999999999999991</v>
       </c>
       <c r="L208" s="2">
@@ -18071,15 +18111,15 @@
         <v>0</v>
       </c>
       <c r="H209">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="I209">
-        <f>D209-C209</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J209">
-        <f>F209-E209</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L209" s="2">
@@ -18106,15 +18146,15 @@
         <v>3.6</v>
       </c>
       <c r="H210">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I210">
-        <f>D210-C210</f>
+        <f t="shared" si="10"/>
         <v>0.8</v>
       </c>
       <c r="J210">
-        <f>F210-E210</f>
+        <f t="shared" si="11"/>
         <v>3.6</v>
       </c>
       <c r="L210" s="2">
@@ -18141,15 +18181,15 @@
         <v>0</v>
       </c>
       <c r="H211">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="I211">
-        <f>D211-C211</f>
+        <f t="shared" si="10"/>
         <v>1.7999999999999972</v>
       </c>
       <c r="J211">
-        <f>F211-E211</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L211" s="2">
@@ -18176,15 +18216,15 @@
         <v>0</v>
       </c>
       <c r="H212">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0.36999999999999988</v>
       </c>
       <c r="I212">
-        <f>D212-C212</f>
+        <f t="shared" si="10"/>
         <v>9.7000000000000028</v>
       </c>
       <c r="J212">
-        <f>F212-E212</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L212" s="2">

</xml_diff>